<commit_message>
May 10th update, deaths lag analysis
</commit_message>
<xml_diff>
--- a/data/NRS_covid_deaths.xlsx
+++ b/data/NRS_covid_deaths.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6495" tabRatio="699"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" tabRatio="699"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="12" r:id="rId1"/>
@@ -1291,7 +1291,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1375,6 +1375,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1411,7 +1422,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="333">
+  <cellXfs count="337">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="11" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1944,10 +1955,6 @@
     </xf>
     <xf numFmtId="3" fontId="10" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="22" fillId="3" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="10" fillId="3" borderId="7" xfId="20" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="10" fillId="3" borderId="0" xfId="20" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1978,15 +1985,6 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="33" fillId="3" borderId="0" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="0" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="7" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="0" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="23" fillId="3" borderId="1" xfId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -2042,6 +2040,7 @@
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="8" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="11" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2052,7 +2051,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="8" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2066,12 +2064,6 @@
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2080,6 +2072,12 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2094,6 +2092,24 @@
     </xf>
     <xf numFmtId="49" fontId="18" fillId="3" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2131,23 +2147,28 @@
     <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="3" fontId="22" fillId="3" borderId="5" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="3" fontId="10" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="0" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="4" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="7" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="0" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="4" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="9" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="24">
@@ -9278,6 +9299,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9724,6 +9746,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9946,6 +9969,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10042,7 +10066,7 @@
           </c:dPt>
           <c:cat>
             <c:numRef>
-              <c:f>'Figure 8 data'!$A$4:$A$56</c:f>
+              <c:f>'Figure 8 data'!$A$6:$A$58</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="53"/>
@@ -10210,7 +10234,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Figure 8 data'!$B$4:$B$56</c:f>
+              <c:f>'Figure 8 data'!$B$6:$B$58</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="53"/>
@@ -10430,7 +10454,7 @@
           </c:dPt>
           <c:cat>
             <c:numRef>
-              <c:f>'Figure 8 data'!$A$4:$A$56</c:f>
+              <c:f>'Figure 8 data'!$A$6:$A$58</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="53"/>
@@ -10598,7 +10622,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Figure 8 data'!$C$4:$C$56</c:f>
+              <c:f>'Figure 8 data'!$C$6:$C$58</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="53"/>
@@ -10886,6 +10910,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -21751,17 +21776,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="275" t="s">
+      <c r="A1" s="270" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="275"/>
-      <c r="C1" s="275"/>
-      <c r="D1" s="275"/>
-      <c r="E1" s="275"/>
-      <c r="F1" s="275"/>
-      <c r="G1" s="275"/>
-      <c r="H1" s="275"/>
-      <c r="I1" s="275"/>
+      <c r="B1" s="270"/>
+      <c r="C1" s="270"/>
+      <c r="D1" s="270"/>
+      <c r="E1" s="270"/>
+      <c r="F1" s="270"/>
+      <c r="G1" s="270"/>
+      <c r="H1" s="270"/>
+      <c r="I1" s="270"/>
       <c r="J1" s="26"/>
       <c r="K1" s="26"/>
       <c r="L1" s="25"/>
@@ -21781,12 +21806,12 @@
       <c r="L2" s="25"/>
     </row>
     <row r="3" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="278" t="s">
+      <c r="A3" s="273" t="s">
         <v>160</v>
       </c>
-      <c r="B3" s="278"/>
-      <c r="C3" s="278"/>
-      <c r="D3" s="278"/>
+      <c r="B3" s="273"/>
+      <c r="C3" s="273"/>
+      <c r="D3" s="273"/>
       <c r="E3" s="26"/>
       <c r="F3" s="26"/>
       <c r="G3" s="26"/>
@@ -21818,20 +21843,20 @@
       <c r="A6" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="277" t="s">
+      <c r="B6" s="272" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="277"/>
-      <c r="D6" s="277"/>
-      <c r="E6" s="277"/>
-      <c r="F6" s="277"/>
-      <c r="G6" s="277"/>
-      <c r="H6" s="277"/>
-      <c r="I6" s="277"/>
-      <c r="J6" s="277"/>
-      <c r="K6" s="277"/>
-      <c r="L6" s="277"/>
-      <c r="M6" s="277"/>
+      <c r="C6" s="272"/>
+      <c r="D6" s="272"/>
+      <c r="E6" s="272"/>
+      <c r="F6" s="272"/>
+      <c r="G6" s="272"/>
+      <c r="H6" s="272"/>
+      <c r="I6" s="272"/>
+      <c r="J6" s="272"/>
+      <c r="K6" s="272"/>
+      <c r="L6" s="272"/>
+      <c r="M6" s="272"/>
       <c r="N6" s="34"/>
       <c r="O6" s="34"/>
       <c r="P6" s="34"/>
@@ -21840,20 +21865,20 @@
       <c r="A7" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="277" t="s">
+      <c r="B7" s="272" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="277"/>
-      <c r="D7" s="277"/>
-      <c r="E7" s="277"/>
-      <c r="F7" s="277"/>
-      <c r="G7" s="277"/>
-      <c r="H7" s="277"/>
-      <c r="I7" s="277"/>
-      <c r="J7" s="277"/>
-      <c r="K7" s="277"/>
-      <c r="L7" s="277"/>
-      <c r="M7" s="277"/>
+      <c r="C7" s="272"/>
+      <c r="D7" s="272"/>
+      <c r="E7" s="272"/>
+      <c r="F7" s="272"/>
+      <c r="G7" s="272"/>
+      <c r="H7" s="272"/>
+      <c r="I7" s="272"/>
+      <c r="J7" s="272"/>
+      <c r="K7" s="272"/>
+      <c r="L7" s="272"/>
+      <c r="M7" s="272"/>
       <c r="N7" s="34"/>
       <c r="O7" s="34"/>
       <c r="P7" s="34"/>
@@ -21862,16 +21887,16 @@
       <c r="A8" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="B8" s="277" t="s">
+      <c r="B8" s="272" t="s">
         <v>134</v>
       </c>
-      <c r="C8" s="277"/>
-      <c r="D8" s="277"/>
-      <c r="E8" s="277"/>
-      <c r="F8" s="277"/>
-      <c r="G8" s="277"/>
-      <c r="H8" s="277"/>
-      <c r="I8" s="277"/>
+      <c r="C8" s="272"/>
+      <c r="D8" s="272"/>
+      <c r="E8" s="272"/>
+      <c r="F8" s="272"/>
+      <c r="G8" s="272"/>
+      <c r="H8" s="272"/>
+      <c r="I8" s="272"/>
       <c r="J8" s="141"/>
       <c r="K8" s="141"/>
       <c r="L8" s="141"/>
@@ -21884,20 +21909,20 @@
       <c r="A9" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="277" t="s">
+      <c r="B9" s="272" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="277"/>
-      <c r="D9" s="277"/>
-      <c r="E9" s="277"/>
-      <c r="F9" s="277"/>
-      <c r="G9" s="277"/>
-      <c r="H9" s="277"/>
-      <c r="I9" s="277"/>
-      <c r="J9" s="277"/>
-      <c r="K9" s="277"/>
-      <c r="L9" s="277"/>
-      <c r="M9" s="277"/>
+      <c r="C9" s="272"/>
+      <c r="D9" s="272"/>
+      <c r="E9" s="272"/>
+      <c r="F9" s="272"/>
+      <c r="G9" s="272"/>
+      <c r="H9" s="272"/>
+      <c r="I9" s="272"/>
+      <c r="J9" s="272"/>
+      <c r="K9" s="272"/>
+      <c r="L9" s="272"/>
+      <c r="M9" s="272"/>
       <c r="N9" s="34"/>
       <c r="O9" s="34"/>
       <c r="P9" s="34"/>
@@ -21906,20 +21931,20 @@
       <c r="A10" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="277" t="s">
+      <c r="B10" s="272" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="277"/>
-      <c r="D10" s="277"/>
-      <c r="E10" s="277"/>
-      <c r="F10" s="277"/>
-      <c r="G10" s="277"/>
-      <c r="H10" s="277"/>
-      <c r="I10" s="277"/>
-      <c r="J10" s="277"/>
-      <c r="K10" s="277"/>
-      <c r="L10" s="277"/>
-      <c r="M10" s="277"/>
+      <c r="C10" s="272"/>
+      <c r="D10" s="272"/>
+      <c r="E10" s="272"/>
+      <c r="F10" s="272"/>
+      <c r="G10" s="272"/>
+      <c r="H10" s="272"/>
+      <c r="I10" s="272"/>
+      <c r="J10" s="272"/>
+      <c r="K10" s="272"/>
+      <c r="L10" s="272"/>
+      <c r="M10" s="272"/>
       <c r="N10" s="34"/>
       <c r="O10" s="34"/>
       <c r="P10" s="34"/>
@@ -21928,20 +21953,20 @@
       <c r="A11" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="277" t="s">
+      <c r="B11" s="272" t="s">
         <v>161</v>
       </c>
-      <c r="C11" s="277"/>
-      <c r="D11" s="277"/>
-      <c r="E11" s="277"/>
-      <c r="F11" s="277"/>
-      <c r="G11" s="277"/>
-      <c r="H11" s="277"/>
-      <c r="I11" s="277"/>
-      <c r="J11" s="277"/>
-      <c r="K11" s="277"/>
-      <c r="L11" s="277"/>
-      <c r="M11" s="277"/>
+      <c r="C11" s="272"/>
+      <c r="D11" s="272"/>
+      <c r="E11" s="272"/>
+      <c r="F11" s="272"/>
+      <c r="G11" s="272"/>
+      <c r="H11" s="272"/>
+      <c r="I11" s="272"/>
+      <c r="J11" s="272"/>
+      <c r="K11" s="272"/>
+      <c r="L11" s="272"/>
+      <c r="M11" s="272"/>
       <c r="N11" s="34"/>
       <c r="O11" s="34"/>
       <c r="P11" s="34"/>
@@ -21950,20 +21975,20 @@
       <c r="A12" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="277" t="s">
+      <c r="B12" s="272" t="s">
         <v>162</v>
       </c>
-      <c r="C12" s="277"/>
-      <c r="D12" s="277"/>
-      <c r="E12" s="277"/>
-      <c r="F12" s="277"/>
-      <c r="G12" s="277"/>
-      <c r="H12" s="277"/>
-      <c r="I12" s="277"/>
-      <c r="J12" s="277"/>
-      <c r="K12" s="277"/>
-      <c r="L12" s="277"/>
-      <c r="M12" s="277"/>
+      <c r="C12" s="272"/>
+      <c r="D12" s="272"/>
+      <c r="E12" s="272"/>
+      <c r="F12" s="272"/>
+      <c r="G12" s="272"/>
+      <c r="H12" s="272"/>
+      <c r="I12" s="272"/>
+      <c r="J12" s="272"/>
+      <c r="K12" s="272"/>
+      <c r="L12" s="272"/>
+      <c r="M12" s="272"/>
       <c r="N12" s="34"/>
       <c r="O12" s="34"/>
       <c r="P12" s="34"/>
@@ -21972,20 +21997,20 @@
       <c r="A13" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="280" t="s">
+      <c r="B13" s="275" t="s">
         <v>163</v>
       </c>
-      <c r="C13" s="280"/>
-      <c r="D13" s="280"/>
-      <c r="E13" s="280"/>
-      <c r="F13" s="280"/>
-      <c r="G13" s="280"/>
-      <c r="H13" s="280"/>
-      <c r="I13" s="280"/>
-      <c r="J13" s="280"/>
-      <c r="K13" s="280"/>
-      <c r="L13" s="280"/>
-      <c r="M13" s="280"/>
+      <c r="C13" s="275"/>
+      <c r="D13" s="275"/>
+      <c r="E13" s="275"/>
+      <c r="F13" s="275"/>
+      <c r="G13" s="275"/>
+      <c r="H13" s="275"/>
+      <c r="I13" s="275"/>
+      <c r="J13" s="275"/>
+      <c r="K13" s="275"/>
+      <c r="L13" s="275"/>
+      <c r="M13" s="275"/>
       <c r="N13" s="34"/>
       <c r="O13" s="34"/>
       <c r="P13" s="34"/>
@@ -21994,20 +22019,20 @@
       <c r="A14" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="277" t="s">
+      <c r="B14" s="272" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="277"/>
-      <c r="D14" s="277"/>
-      <c r="E14" s="277"/>
-      <c r="F14" s="277"/>
-      <c r="G14" s="277"/>
-      <c r="H14" s="277"/>
-      <c r="I14" s="277"/>
-      <c r="J14" s="277"/>
-      <c r="K14" s="277"/>
-      <c r="L14" s="277"/>
-      <c r="M14" s="277"/>
+      <c r="C14" s="272"/>
+      <c r="D14" s="272"/>
+      <c r="E14" s="272"/>
+      <c r="F14" s="272"/>
+      <c r="G14" s="272"/>
+      <c r="H14" s="272"/>
+      <c r="I14" s="272"/>
+      <c r="J14" s="272"/>
+      <c r="K14" s="272"/>
+      <c r="L14" s="272"/>
+      <c r="M14" s="272"/>
       <c r="N14" s="34"/>
       <c r="O14" s="34"/>
       <c r="P14" s="34"/>
@@ -22016,15 +22041,15 @@
       <c r="A15" s="156" t="s">
         <v>147</v>
       </c>
-      <c r="B15" s="277" t="s">
+      <c r="B15" s="272" t="s">
         <v>164</v>
       </c>
-      <c r="C15" s="277"/>
-      <c r="D15" s="277"/>
-      <c r="E15" s="277"/>
-      <c r="F15" s="277"/>
-      <c r="G15" s="277"/>
-      <c r="H15" s="277"/>
+      <c r="C15" s="272"/>
+      <c r="D15" s="272"/>
+      <c r="E15" s="272"/>
+      <c r="F15" s="272"/>
+      <c r="G15" s="272"/>
+      <c r="H15" s="272"/>
       <c r="I15" s="155"/>
       <c r="J15" s="155"/>
       <c r="K15" s="155"/>
@@ -22038,20 +22063,20 @@
       <c r="A16" s="115" t="s">
         <v>136</v>
       </c>
-      <c r="B16" s="277" t="s">
+      <c r="B16" s="272" t="s">
         <v>176</v>
       </c>
-      <c r="C16" s="277"/>
-      <c r="D16" s="277"/>
-      <c r="E16" s="277"/>
-      <c r="F16" s="277"/>
-      <c r="G16" s="277"/>
-      <c r="H16" s="277"/>
-      <c r="I16" s="277"/>
-      <c r="J16" s="277"/>
-      <c r="K16" s="277"/>
-      <c r="L16" s="277"/>
-      <c r="M16" s="277"/>
+      <c r="C16" s="272"/>
+      <c r="D16" s="272"/>
+      <c r="E16" s="272"/>
+      <c r="F16" s="272"/>
+      <c r="G16" s="272"/>
+      <c r="H16" s="272"/>
+      <c r="I16" s="272"/>
+      <c r="J16" s="272"/>
+      <c r="K16" s="272"/>
+      <c r="L16" s="272"/>
+      <c r="M16" s="272"/>
       <c r="N16" s="34"/>
       <c r="O16" s="34"/>
       <c r="P16" s="34"/>
@@ -22060,20 +22085,20 @@
       <c r="A17" s="233" t="s">
         <v>175</v>
       </c>
-      <c r="B17" s="277" t="s">
+      <c r="B17" s="272" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="277"/>
-      <c r="D17" s="277"/>
-      <c r="E17" s="277"/>
-      <c r="F17" s="277"/>
-      <c r="G17" s="277"/>
-      <c r="H17" s="277"/>
-      <c r="I17" s="277"/>
-      <c r="J17" s="277"/>
-      <c r="K17" s="277"/>
-      <c r="L17" s="277"/>
-      <c r="M17" s="277"/>
+      <c r="C17" s="272"/>
+      <c r="D17" s="272"/>
+      <c r="E17" s="272"/>
+      <c r="F17" s="272"/>
+      <c r="G17" s="272"/>
+      <c r="H17" s="272"/>
+      <c r="I17" s="272"/>
+      <c r="J17" s="272"/>
+      <c r="K17" s="272"/>
+      <c r="L17" s="272"/>
+      <c r="M17" s="272"/>
       <c r="N17" s="34"/>
       <c r="O17" s="34"/>
       <c r="P17" s="34"/>
@@ -22097,15 +22122,15 @@
       <c r="P18" s="34"/>
     </row>
     <row r="19" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="279" t="s">
+      <c r="A19" s="274" t="s">
         <v>214</v>
       </c>
-      <c r="B19" s="279"/>
-      <c r="C19" s="279"/>
-      <c r="D19" s="279"/>
-      <c r="E19" s="279"/>
-      <c r="F19" s="279"/>
-      <c r="G19" s="279"/>
+      <c r="B19" s="274"/>
+      <c r="C19" s="274"/>
+      <c r="D19" s="274"/>
+      <c r="E19" s="274"/>
+      <c r="F19" s="274"/>
+      <c r="G19" s="274"/>
       <c r="H19" s="34"/>
       <c r="I19" s="34"/>
       <c r="J19" s="34"/>
@@ -22117,10 +22142,10 @@
       <c r="P19" s="34"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="276" t="s">
+      <c r="A21" s="271" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="276"/>
+      <c r="B21" s="271"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -22178,22 +22203,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="322" t="s">
+      <c r="A1" s="323" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="322"/>
-      <c r="C1" s="322"/>
-      <c r="D1" s="322"/>
-      <c r="E1" s="322"/>
-      <c r="F1" s="322"/>
-      <c r="G1" s="322"/>
-      <c r="H1" s="322"/>
-      <c r="I1" s="322"/>
-      <c r="K1" s="324" t="s">
+      <c r="B1" s="323"/>
+      <c r="C1" s="323"/>
+      <c r="D1" s="323"/>
+      <c r="E1" s="323"/>
+      <c r="F1" s="323"/>
+      <c r="G1" s="323"/>
+      <c r="H1" s="323"/>
+      <c r="I1" s="323"/>
+      <c r="K1" s="325" t="s">
         <v>70</v>
       </c>
-      <c r="L1" s="324"/>
-      <c r="M1" s="324"/>
+      <c r="L1" s="325"/>
+      <c r="M1" s="325"/>
       <c r="N1" s="172"/>
       <c r="O1" s="172"/>
     </row>
@@ -23067,7 +23092,7 @@
       <c r="S18" s="229">
         <v>1673</v>
       </c>
-      <c r="U18" s="251"/>
+      <c r="U18" s="249"/>
     </row>
     <row r="19" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="180" t="s">
@@ -23168,7 +23193,7 @@
         <f>S12-S5</f>
         <v>-4</v>
       </c>
-      <c r="T20" s="251"/>
+      <c r="T20" s="249"/>
     </row>
     <row r="21" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="176" t="s">
@@ -23246,7 +23271,7 @@
         <f t="shared" si="5"/>
         <v>43</v>
       </c>
-      <c r="T21" s="251"/>
+      <c r="T21" s="249"/>
     </row>
     <row r="22" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="176" t="s">
@@ -23324,7 +23349,7 @@
         <f t="shared" si="8"/>
         <v>50</v>
       </c>
-      <c r="T22" s="251"/>
+      <c r="T22" s="249"/>
     </row>
     <row r="23" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="176" t="s">
@@ -23402,7 +23427,7 @@
         <f t="shared" si="11"/>
         <v>-19</v>
       </c>
-      <c r="T23" s="251"/>
+      <c r="T23" s="249"/>
     </row>
     <row r="24" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="176" t="s">
@@ -23480,7 +23505,7 @@
         <f t="shared" si="14"/>
         <v>495</v>
       </c>
-      <c r="T24" s="251"/>
+      <c r="T24" s="249"/>
     </row>
     <row r="25" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="176" t="s">
@@ -23558,7 +23583,7 @@
         <f t="shared" si="16"/>
         <v>28</v>
       </c>
-      <c r="T25" s="251"/>
+      <c r="T25" s="249"/>
     </row>
     <row r="26" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="176" t="s">
@@ -23636,62 +23661,62 @@
         <f t="shared" si="18"/>
         <v>594</v>
       </c>
-      <c r="T26" s="251"/>
+      <c r="T26" s="249"/>
     </row>
     <row r="27" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="179"/>
     </row>
     <row r="29" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="261" t="s">
+      <c r="A29" s="259" t="s">
         <v>213</v>
       </c>
-      <c r="B29" s="262"/>
-      <c r="C29" s="262"/>
+      <c r="B29" s="260"/>
+      <c r="C29" s="260"/>
     </row>
     <row r="30" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="323" t="s">
+      <c r="A30" s="324" t="s">
         <v>158</v>
       </c>
-      <c r="B30" s="323"/>
-      <c r="C30" s="323"/>
+      <c r="B30" s="324"/>
+      <c r="C30" s="324"/>
     </row>
     <row r="31" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="260" t="s">
+      <c r="A31" s="258" t="s">
         <v>153</v>
       </c>
-      <c r="B31" s="262"/>
-      <c r="C31" s="262"/>
+      <c r="B31" s="260"/>
+      <c r="C31" s="260"/>
     </row>
     <row r="32" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="323" t="s">
+      <c r="A32" s="324" t="s">
         <v>154</v>
       </c>
-      <c r="B32" s="323"/>
-      <c r="C32" s="262"/>
+      <c r="B32" s="324"/>
+      <c r="C32" s="260"/>
     </row>
     <row r="33" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="260" t="s">
+      <c r="A33" s="258" t="s">
         <v>155</v>
       </c>
-      <c r="B33" s="262"/>
-      <c r="C33" s="262"/>
+      <c r="B33" s="260"/>
+      <c r="C33" s="260"/>
     </row>
     <row r="34" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="260" t="s">
+      <c r="A34" s="258" t="s">
         <v>156</v>
       </c>
-      <c r="B34" s="262"/>
-      <c r="C34" s="262"/>
+      <c r="B34" s="260"/>
+      <c r="C34" s="260"/>
     </row>
     <row r="35" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="260" t="s">
+      <c r="A35" s="258" t="s">
         <v>157</v>
       </c>
-      <c r="B35" s="262"/>
-      <c r="C35" s="262"/>
+      <c r="B35" s="260"/>
+      <c r="C35" s="260"/>
     </row>
     <row r="37" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="260" t="s">
+      <c r="A37" s="258" t="s">
         <v>150</v>
       </c>
     </row>
@@ -23712,7 +23737,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
@@ -23725,24 +23750,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="325" t="s">
+      <c r="A1" s="326" t="s">
         <v>173</v>
       </c>
-      <c r="B1" s="325"/>
-      <c r="C1" s="325"/>
-      <c r="D1" s="325"/>
-      <c r="E1" s="325"/>
-      <c r="F1" s="325"/>
-      <c r="G1" s="325"/>
-      <c r="H1" s="325"/>
+      <c r="B1" s="326"/>
+      <c r="C1" s="326"/>
+      <c r="D1" s="326"/>
+      <c r="E1" s="326"/>
+      <c r="F1" s="326"/>
+      <c r="G1" s="326"/>
+      <c r="H1" s="326"/>
       <c r="I1" s="177"/>
-      <c r="J1" s="296" t="s">
+      <c r="J1" s="287" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="296"/>
+      <c r="K1" s="287"/>
       <c r="L1" s="177"/>
     </row>
-    <row r="2" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="234"/>
       <c r="C2" s="234"/>
       <c r="D2" s="234"/>
@@ -23953,159 +23978,171 @@
         <v>523</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="246" t="s">
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="328" t="s">
         <v>171</v>
       </c>
-      <c r="B10" s="247"/>
-      <c r="C10" s="234"/>
-      <c r="D10" s="234"/>
-      <c r="E10" s="234"/>
-      <c r="F10" s="234"/>
-      <c r="G10" s="234"/>
-      <c r="H10" s="234"/>
+      <c r="B10" s="329"/>
+      <c r="C10" s="330"/>
+      <c r="D10" s="330"/>
+      <c r="E10" s="330"/>
+      <c r="F10" s="330"/>
+      <c r="G10" s="330"/>
+      <c r="H10" s="330"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="241" t="s">
+      <c r="A11" s="328"/>
+      <c r="B11" s="329"/>
+      <c r="C11" s="330"/>
+      <c r="D11" s="330"/>
+      <c r="E11" s="330"/>
+      <c r="F11" s="330"/>
+      <c r="G11" s="330"/>
+      <c r="H11" s="330"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="241" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="248">
+      <c r="B12" s="246">
         <f>B5/B$9</f>
         <v>0</v>
       </c>
-      <c r="C11" s="249">
-        <f t="shared" ref="C11:G11" si="2">C5/C$9</f>
+      <c r="C12" s="247">
+        <f t="shared" ref="C12:G12" si="2">C5/C$9</f>
         <v>8.0645161290322578E-2</v>
       </c>
-      <c r="D11" s="249">
+      <c r="D12" s="247">
         <f t="shared" si="2"/>
         <v>0.17375886524822695</v>
       </c>
-      <c r="E11" s="249">
+      <c r="E12" s="247">
         <f t="shared" si="2"/>
         <v>0.30983606557377047</v>
       </c>
-      <c r="F11" s="249">
+      <c r="F12" s="247">
         <f t="shared" si="2"/>
         <v>0.46615384615384614</v>
       </c>
-      <c r="G11" s="249">
+      <c r="G12" s="247">
         <f t="shared" si="2"/>
         <v>0.51519756838905773</v>
       </c>
-      <c r="H11" s="249">
-        <f t="shared" ref="H11" si="3">H5/H$9</f>
+      <c r="H12" s="247">
+        <f t="shared" ref="H12" si="3">H5/H$9</f>
         <v>0.59273422562141487</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="241" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="241" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="248">
-        <f t="shared" ref="B12:G12" si="4">B6/B$9</f>
+      <c r="B13" s="246">
+        <f t="shared" ref="B13:G13" si="4">B6/B$9</f>
         <v>0.2</v>
       </c>
-      <c r="C12" s="249">
+      <c r="C13" s="247">
         <f t="shared" si="4"/>
         <v>0.22580645161290322</v>
       </c>
-      <c r="D12" s="249">
+      <c r="D13" s="247">
         <f t="shared" si="4"/>
         <v>0.13829787234042554</v>
       </c>
-      <c r="E12" s="249">
+      <c r="E13" s="247">
         <f t="shared" si="4"/>
         <v>0.10491803278688525</v>
       </c>
-      <c r="F12" s="249">
+      <c r="F13" s="247">
         <f t="shared" si="4"/>
         <v>5.5384615384615386E-2</v>
       </c>
-      <c r="G12" s="249">
+      <c r="G13" s="247">
         <f t="shared" si="4"/>
         <v>6.3829787234042548E-2</v>
       </c>
-      <c r="H12" s="249">
-        <f t="shared" ref="H12" si="5">H6/H$9</f>
+      <c r="H13" s="247">
+        <f t="shared" ref="H13" si="5">H6/H$9</f>
         <v>3.6328871892925434E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="241" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="241" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="248">
-        <f t="shared" ref="B13:G13" si="6">B7/B$9</f>
+      <c r="B14" s="246">
+        <f t="shared" ref="B14:G14" si="6">B7/B$9</f>
         <v>0.8</v>
       </c>
-      <c r="C13" s="249">
+      <c r="C14" s="247">
         <f t="shared" si="6"/>
         <v>0.69354838709677424</v>
       </c>
-      <c r="D13" s="249">
+      <c r="D14" s="247">
         <f t="shared" si="6"/>
         <v>0.68439716312056742</v>
       </c>
-      <c r="E13" s="249">
+      <c r="E14" s="247">
         <f t="shared" si="6"/>
         <v>0.58524590163934431</v>
       </c>
-      <c r="F13" s="249">
+      <c r="F14" s="247">
         <f t="shared" si="6"/>
         <v>0.47846153846153844</v>
       </c>
-      <c r="G13" s="249">
+      <c r="G14" s="247">
         <f t="shared" si="6"/>
         <v>0.42097264437689969</v>
       </c>
-      <c r="H13" s="249">
-        <f t="shared" ref="H13" si="7">H7/H$9</f>
+      <c r="H14" s="247">
+        <f t="shared" ref="H14" si="7">H7/H$9</f>
         <v>0.37093690248565964</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="241" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="241" t="s">
         <v>84</v>
       </c>
-      <c r="B14" s="248">
-        <f t="shared" ref="B14:G14" si="8">B8/B$9</f>
-        <v>0</v>
-      </c>
-      <c r="C14" s="249">
+      <c r="B15" s="246">
+        <f t="shared" ref="B15:G15" si="8">B8/B$9</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="247">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="D14" s="249">
+      <c r="D15" s="247">
         <f t="shared" si="8"/>
         <v>3.5460992907801418E-3</v>
       </c>
-      <c r="E14" s="249">
+      <c r="E15" s="247">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="F14" s="249">
+      <c r="F15" s="247">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="G14" s="249">
+      <c r="G15" s="247">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="H14" s="249">
-        <f t="shared" ref="H14" si="9">H8/H$9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="263" t="s">
+      <c r="H15" s="247">
+        <f t="shared" ref="H15" si="9">H8/H$9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="261" t="s">
         <v>150</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="J1:K1"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:H11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J1" location="Contents!A1" display="back to contents"/>
@@ -24117,7 +24154,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
@@ -24132,665 +24169,678 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="326" t="s">
+      <c r="A1" s="327" t="s">
         <v>172</v>
       </c>
-      <c r="B1" s="326"/>
-      <c r="C1" s="326"/>
-      <c r="D1" s="326"/>
-      <c r="E1" s="326"/>
-      <c r="F1" s="326"/>
-      <c r="G1" s="326"/>
-      <c r="I1" s="316" t="s">
+      <c r="B1" s="327"/>
+      <c r="C1" s="327"/>
+      <c r="D1" s="327"/>
+      <c r="E1" s="327"/>
+      <c r="F1" s="327"/>
+      <c r="G1" s="327"/>
+      <c r="I1" s="317" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="316"/>
+      <c r="J1" s="317"/>
     </row>
     <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="119"/>
     </row>
-    <row r="3" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="265" t="s">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="331" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="266" t="s">
+      <c r="B3" s="333" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="267" t="s">
+      <c r="C3" s="334" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="268">
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="331"/>
+      <c r="B4" s="333"/>
+      <c r="C4" s="334"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="332"/>
+      <c r="B5" s="336"/>
+      <c r="C5" s="335"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="263">
         <v>43902</v>
       </c>
-      <c r="B4" s="269">
+      <c r="B6" s="264">
         <v>2</v>
       </c>
-      <c r="C4" s="270">
+      <c r="C6" s="265">
         <f>'Figure 2 data'!B4</f>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="271">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="266">
         <v>43903</v>
       </c>
-      <c r="B5" s="272">
+      <c r="B7" s="267">
         <v>2</v>
       </c>
-      <c r="C5" s="273">
+      <c r="C7" s="268">
         <f>'Figure 2 data'!B56</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="271">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="266">
         <v>43904</v>
       </c>
-      <c r="B6" s="272">
+      <c r="B8" s="267">
         <v>4</v>
       </c>
-      <c r="C6" s="273">
+      <c r="C8" s="268">
         <f>'Figure 2 data'!B57</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="271">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="266">
         <v>43905</v>
       </c>
-      <c r="B7" s="272">
+      <c r="B9" s="267">
         <v>5</v>
       </c>
-      <c r="C7" s="273">
+      <c r="C9" s="268">
         <f>'Figure 2 data'!B58</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="271">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="266">
         <v>43906</v>
       </c>
-      <c r="B8" s="272">
+      <c r="B10" s="267">
         <v>8</v>
       </c>
-      <c r="C8" s="273">
+      <c r="C10" s="268">
         <f>'Figure 2 data'!B59</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="271">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="266">
         <v>43907</v>
       </c>
-      <c r="B9" s="272">
+      <c r="B11" s="267">
         <v>10</v>
       </c>
-      <c r="C9" s="273">
+      <c r="C11" s="268">
         <f>'Figure 2 data'!B60</f>
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="271">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="266">
         <v>43908</v>
       </c>
-      <c r="B10" s="272">
+      <c r="B12" s="267">
         <v>14</v>
       </c>
-      <c r="C10" s="273">
+      <c r="C12" s="268">
         <f>'Figure 2 data'!B61</f>
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="271">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="266">
         <v>43909</v>
       </c>
-      <c r="B11" s="272">
+      <c r="B13" s="267">
         <v>18</v>
       </c>
-      <c r="C11" s="273">
+      <c r="C13" s="268">
         <f>'Figure 2 data'!B62</f>
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="271">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="266">
         <v>43910</v>
       </c>
-      <c r="B12" s="272">
+      <c r="B14" s="267">
         <v>23</v>
       </c>
-      <c r="C12" s="273">
+      <c r="C14" s="268">
         <f>'Figure 2 data'!B63</f>
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="271">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="266">
         <v>43911</v>
       </c>
-      <c r="B13" s="272">
+      <c r="B15" s="267">
         <v>30</v>
       </c>
-      <c r="C13" s="273">
+      <c r="C15" s="268">
         <f>'Figure 2 data'!B64</f>
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="271">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="266">
         <v>43912</v>
       </c>
-      <c r="B14" s="272">
+      <c r="B16" s="267">
         <v>36</v>
       </c>
-      <c r="C14" s="273">
+      <c r="C16" s="268">
         <f>'Figure 2 data'!B65</f>
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="271">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="266">
         <v>43913</v>
       </c>
-      <c r="B15" s="272">
+      <c r="B17" s="267">
         <v>43</v>
       </c>
-      <c r="C15" s="273">
+      <c r="C17" s="268">
         <f>'Figure 2 data'!B66</f>
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="271">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="266">
         <v>43914</v>
       </c>
-      <c r="B16" s="272">
+      <c r="B18" s="267">
         <v>55</v>
       </c>
-      <c r="C16" s="273">
+      <c r="C18" s="268">
         <f>'Figure 2 data'!B67</f>
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="271">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="266">
         <v>43915</v>
       </c>
-      <c r="B17" s="272">
+      <c r="B19" s="267">
         <v>77</v>
       </c>
-      <c r="C17" s="273">
+      <c r="C19" s="268">
         <f>'Figure 2 data'!B68</f>
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="271">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="266">
         <v>43916</v>
       </c>
-      <c r="B18" s="272">
+      <c r="B20" s="267">
         <v>100</v>
       </c>
-      <c r="C18" s="273">
+      <c r="C20" s="268">
         <f>'Figure 2 data'!B69</f>
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="271">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="266">
         <v>43917</v>
       </c>
-      <c r="B19" s="272">
+      <c r="B21" s="267">
         <v>123</v>
       </c>
-      <c r="C19" s="273">
+      <c r="C21" s="268">
         <f>'Figure 2 data'!B70</f>
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="271">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="266">
         <v>43918</v>
       </c>
-      <c r="B20" s="272">
+      <c r="B22" s="267">
         <v>160</v>
       </c>
-      <c r="C20" s="273">
+      <c r="C22" s="268">
         <f>'Figure 2 data'!B71</f>
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="271">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="266">
         <v>43919</v>
       </c>
-      <c r="B21" s="272">
+      <c r="B23" s="267">
         <v>187</v>
       </c>
-      <c r="C21" s="273">
+      <c r="C23" s="268">
         <f>'Figure 2 data'!B72</f>
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="271">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="266">
         <v>43920</v>
       </c>
-      <c r="B22" s="272">
+      <c r="B24" s="267">
         <v>238</v>
       </c>
-      <c r="C22" s="273">
+      <c r="C24" s="268">
         <f>'Figure 2 data'!B73</f>
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="271">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="266">
         <v>43921</v>
       </c>
-      <c r="B23" s="272">
+      <c r="B25" s="267">
         <v>296</v>
       </c>
-      <c r="C23" s="273">
+      <c r="C25" s="268">
         <f>'Figure 2 data'!B74</f>
         <v>165</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="271">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="266">
         <v>43922</v>
       </c>
-      <c r="B24" s="272">
+      <c r="B26" s="267">
         <v>361</v>
       </c>
-      <c r="C24" s="273">
+      <c r="C26" s="268">
         <f>'Figure 2 data'!B75</f>
         <v>214</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="271">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="266">
         <v>43923</v>
       </c>
-      <c r="B25" s="272">
+      <c r="B27" s="267">
         <v>422</v>
       </c>
-      <c r="C25" s="273">
+      <c r="C27" s="268">
         <f>'Figure 2 data'!B76</f>
         <v>277</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="271">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="266">
         <v>43924</v>
       </c>
-      <c r="B26" s="272">
+      <c r="B28" s="267">
         <v>498</v>
       </c>
-      <c r="C26" s="273">
+      <c r="C28" s="268">
         <f>'Figure 2 data'!B77</f>
         <v>348</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="271">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="266">
         <v>43925</v>
       </c>
-      <c r="B27" s="272">
+      <c r="B29" s="267">
         <v>554</v>
       </c>
-      <c r="C27" s="273">
+      <c r="C29" s="268">
         <f>'Figure 2 data'!B78</f>
         <v>350</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="271">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="266">
         <v>43926</v>
       </c>
-      <c r="B28" s="272">
+      <c r="B30" s="267">
         <v>640</v>
       </c>
-      <c r="C28" s="273">
+      <c r="C30" s="268">
         <f>'Figure 2 data'!B79</f>
         <v>354</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="271">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="266">
         <v>43927</v>
       </c>
-      <c r="B29" s="272">
+      <c r="B31" s="267">
         <v>729</v>
       </c>
-      <c r="C29" s="273">
+      <c r="C31" s="268">
         <f>'Figure 2 data'!B80</f>
         <v>476</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="271">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="266">
         <v>43928</v>
       </c>
-      <c r="B30" s="272">
+      <c r="B32" s="267">
         <v>813</v>
       </c>
-      <c r="C30" s="273">
+      <c r="C32" s="268">
         <f>'Figure 2 data'!B81</f>
         <v>593</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="271">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="266">
         <v>43929</v>
       </c>
-      <c r="B31" s="272">
+      <c r="B33" s="267">
         <v>904</v>
       </c>
-      <c r="C31" s="273">
+      <c r="C33" s="268">
         <f>'Figure 2 data'!B82</f>
         <v>718</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="271">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="266">
         <v>43930</v>
       </c>
-      <c r="B32" s="272">
+      <c r="B34" s="267">
         <v>1012</v>
       </c>
-      <c r="C32" s="273">
+      <c r="C34" s="268">
         <f>'Figure 2 data'!B83</f>
         <v>819</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="271">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="266">
         <v>43931</v>
       </c>
-      <c r="B33" s="272">
+      <c r="B35" s="267">
         <v>1110</v>
       </c>
-      <c r="C33" s="273">
+      <c r="C35" s="268">
         <f>'Figure 2 data'!B84</f>
         <v>904</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="274">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="269">
         <v>43932</v>
       </c>
-      <c r="B34" s="272">
+      <c r="B36" s="267">
         <v>1205</v>
       </c>
-      <c r="C34" s="273">
+      <c r="C36" s="268">
         <f>'Figure 2 data'!B85</f>
         <v>954</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="274">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="269">
         <v>43933</v>
       </c>
-      <c r="B35" s="272">
+      <c r="B37" s="267">
         <v>1279</v>
       </c>
-      <c r="C35" s="273">
+      <c r="C37" s="268">
         <f>'Figure 2 data'!B86</f>
         <v>964</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="274">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="269">
         <v>43934</v>
       </c>
-      <c r="B36" s="273">
+      <c r="B38" s="268">
         <v>1358</v>
       </c>
-      <c r="C36" s="273">
+      <c r="C38" s="268">
         <f>'Figure 2 data'!B87</f>
         <v>1041</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="274">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="269">
         <v>43935</v>
       </c>
-      <c r="B37" s="273">
+      <c r="B39" s="268">
         <v>1458</v>
       </c>
-      <c r="C37" s="273">
+      <c r="C39" s="268">
         <f>'Figure 2 data'!B88</f>
         <v>1185</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="274">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="269">
         <v>43936</v>
       </c>
-      <c r="B38" s="273">
+      <c r="B40" s="268">
         <v>1552</v>
       </c>
-      <c r="C38" s="273">
+      <c r="C40" s="268">
         <f>'Figure 2 data'!B89</f>
         <v>1334</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="274">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="269">
         <v>43937</v>
       </c>
-      <c r="B39" s="273">
+      <c r="B41" s="268">
         <v>1653</v>
       </c>
-      <c r="C39" s="273">
+      <c r="C41" s="268">
         <f>'Figure 2 data'!B90</f>
         <v>1462</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="274">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="269">
         <v>43938</v>
       </c>
-      <c r="B40" s="273">
+      <c r="B42" s="268">
         <v>1738</v>
       </c>
-      <c r="C40" s="273">
+      <c r="C42" s="268">
         <f>'Figure 2 data'!B91</f>
         <v>1572</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="274">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="269">
         <v>43939</v>
       </c>
-      <c r="B41" s="273">
+      <c r="B43" s="268">
         <v>1833</v>
       </c>
-      <c r="C41" s="273">
+      <c r="C43" s="268">
         <f>'Figure 2 data'!B92</f>
         <v>1597</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="274">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="269">
         <v>43940</v>
       </c>
-      <c r="B42" s="273">
+      <c r="B44" s="268">
         <v>1922</v>
       </c>
-      <c r="C42" s="273">
+      <c r="C44" s="268">
         <f>'Figure 2 data'!B93</f>
         <v>1614</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="274">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="269">
         <v>43941</v>
       </c>
-      <c r="B43" s="273">
+      <c r="B45" s="268">
         <v>2027</v>
       </c>
-      <c r="C43" s="273">
+      <c r="C45" s="268">
         <f>'Figure 2 data'!B94</f>
         <v>1738</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="274">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="269">
         <v>43942</v>
       </c>
-      <c r="B44" s="273">
+      <c r="B46" s="268">
         <v>2123</v>
       </c>
-      <c r="C44" s="273">
+      <c r="C46" s="268">
         <f>'Figure 2 data'!B95</f>
         <v>1898</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="274">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="269">
         <v>43943</v>
       </c>
-      <c r="B45" s="273">
+      <c r="B47" s="268">
         <v>2210</v>
       </c>
-      <c r="C45" s="273">
+      <c r="C47" s="268">
         <f>'Figure 2 data'!B96</f>
         <v>2019</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="274">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="269">
         <v>43944</v>
       </c>
-      <c r="B46" s="273">
+      <c r="B48" s="268">
         <v>2282</v>
       </c>
-      <c r="C46" s="273">
+      <c r="C48" s="268">
         <f>'Figure 2 data'!B97</f>
         <v>2134</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="274">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="269">
         <v>43945</v>
       </c>
-      <c r="B47" s="273">
+      <c r="B49" s="268">
         <v>2356</v>
       </c>
-      <c r="C47" s="273">
+      <c r="C49" s="268">
         <f>'Figure 2 data'!B98</f>
         <v>2218</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="274">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="269">
         <v>43946</v>
       </c>
-      <c r="B48" s="273">
+      <c r="B50" s="268">
         <v>2434</v>
       </c>
-      <c r="C48" s="273">
+      <c r="C50" s="268">
         <f>'Figure 2 data'!B99</f>
         <v>2258</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="274">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="269">
         <v>43947</v>
       </c>
-      <c r="B49" s="273">
+      <c r="B51" s="268">
         <v>2511</v>
       </c>
-      <c r="C49" s="273">
+      <c r="C51" s="268">
         <f>'Figure 2 data'!B100</f>
         <v>2272</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="274">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="269">
         <v>43948</v>
       </c>
-      <c r="B50" s="273"/>
-      <c r="C50" s="273">
+      <c r="B52" s="268"/>
+      <c r="C52" s="268">
         <f>'Figure 2 data'!B101</f>
         <v>2380</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="274">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="269">
         <v>43949</v>
       </c>
-      <c r="B51" s="273"/>
-      <c r="C51" s="273">
+      <c r="B53" s="268"/>
+      <c r="C53" s="268">
         <f>'Figure 2 data'!B102</f>
         <v>2514</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="274">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="269">
         <v>43950</v>
       </c>
-      <c r="B52" s="273"/>
-      <c r="C52" s="273">
+      <c r="B54" s="268"/>
+      <c r="C54" s="268">
         <f>'Figure 2 data'!B103</f>
         <v>2626</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="274">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="269">
         <v>43951</v>
       </c>
-      <c r="B53" s="273"/>
-      <c r="C53" s="273">
+      <c r="B55" s="268"/>
+      <c r="C55" s="268">
         <f>'Figure 2 data'!B104</f>
         <v>2699</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="274">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="269">
         <v>43952</v>
       </c>
-      <c r="B54" s="273"/>
-      <c r="C54" s="273">
+      <c r="B56" s="268"/>
+      <c r="C56" s="268">
         <f>'Figure 2 data'!B105</f>
         <v>2774</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="274">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="269">
         <v>43953</v>
       </c>
-      <c r="B55" s="273"/>
-      <c r="C55" s="273">
+      <c r="B57" s="268"/>
+      <c r="C57" s="268">
         <f>'Figure 2 data'!B106</f>
         <v>2788</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="274">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="269">
         <v>43954</v>
       </c>
-      <c r="B56" s="273"/>
-      <c r="C56" s="273">
+      <c r="B58" s="268"/>
+      <c r="C58" s="268">
         <f>'Figure 2 data'!B107</f>
         <v>2795</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="264" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="262" t="s">
         <v>150</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I1" location="Contents!A1" display="back to contents"/>
@@ -24824,42 +24874,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="283" t="s">
+      <c r="A1" s="278" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="283"/>
-      <c r="C1" s="283"/>
-      <c r="D1" s="283"/>
-      <c r="E1" s="283"/>
-      <c r="F1" s="283"/>
-      <c r="G1" s="283"/>
-      <c r="H1" s="283"/>
-      <c r="I1" s="283"/>
-      <c r="J1" s="283"/>
-      <c r="K1" s="283"/>
-      <c r="L1" s="283"/>
-      <c r="M1" s="283"/>
-      <c r="N1" s="283"/>
-      <c r="O1" s="256"/>
-      <c r="P1" s="296" t="s">
+      <c r="B1" s="278"/>
+      <c r="C1" s="278"/>
+      <c r="D1" s="278"/>
+      <c r="E1" s="278"/>
+      <c r="F1" s="278"/>
+      <c r="G1" s="278"/>
+      <c r="H1" s="278"/>
+      <c r="I1" s="278"/>
+      <c r="J1" s="278"/>
+      <c r="K1" s="278"/>
+      <c r="L1" s="278"/>
+      <c r="M1" s="278"/>
+      <c r="N1" s="278"/>
+      <c r="O1" s="254"/>
+      <c r="P1" s="287" t="s">
         <v>70</v>
       </c>
-      <c r="Q1" s="296"/>
+      <c r="Q1" s="287"/>
       <c r="R1" s="184"/>
       <c r="S1" s="197"/>
     </row>
     <row r="2" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="295"/>
-      <c r="B2" s="295"/>
-      <c r="C2" s="295"/>
-      <c r="D2" s="295"/>
-      <c r="E2" s="295"/>
-      <c r="F2" s="295"/>
-      <c r="G2" s="295"/>
-      <c r="H2" s="295"/>
-      <c r="I2" s="295"/>
-      <c r="J2" s="295"/>
-      <c r="K2" s="295"/>
+      <c r="A2" s="291"/>
+      <c r="B2" s="291"/>
+      <c r="C2" s="291"/>
+      <c r="D2" s="291"/>
+      <c r="E2" s="291"/>
+      <c r="F2" s="291"/>
+      <c r="G2" s="291"/>
+      <c r="H2" s="291"/>
+      <c r="I2" s="291"/>
+      <c r="J2" s="291"/>
+      <c r="K2" s="291"/>
       <c r="L2" s="13"/>
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
@@ -24871,10 +24921,10 @@
       <c r="T2" s="13"/>
     </row>
     <row r="3" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="284" t="s">
+      <c r="A3" s="279" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="284"/>
+      <c r="B3" s="279"/>
       <c r="C3" s="5">
         <v>1</v>
       </c>
@@ -24929,14 +24979,14 @@
       <c r="T3" s="185">
         <v>18</v>
       </c>
-      <c r="U3" s="292"/>
-      <c r="V3" s="292"/>
+      <c r="U3" s="288"/>
+      <c r="V3" s="288"/>
     </row>
     <row r="4" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="285" t="s">
+      <c r="A4" s="280" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="285"/>
+      <c r="B4" s="280"/>
       <c r="C4" s="6">
         <v>43829</v>
       </c>
@@ -24991,10 +25041,10 @@
       <c r="T4" s="6">
         <v>43948</v>
       </c>
-      <c r="U4" s="293" t="s">
+      <c r="U4" s="289" t="s">
         <v>27</v>
       </c>
-      <c r="V4" s="293"/>
+      <c r="V4" s="289"/>
     </row>
     <row r="5" spans="1:24" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
@@ -25043,10 +25093,10 @@
       <c r="T6" s="74"/>
     </row>
     <row r="7" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="286" t="s">
+      <c r="A7" s="281" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="286"/>
+      <c r="B7" s="281"/>
       <c r="C7" s="202">
         <v>0</v>
       </c>
@@ -25109,10 +25159,10 @@
       <c r="W7" s="43"/>
     </row>
     <row r="8" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="286" t="s">
+      <c r="A8" s="281" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="286"/>
+      <c r="B8" s="281"/>
       <c r="C8" s="202">
         <f>SUM(C21:C27)</f>
         <v>0</v>
@@ -25193,10 +25243,10 @@
       <c r="W8" s="170"/>
     </row>
     <row r="9" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="286" t="s">
+      <c r="A9" s="281" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="286"/>
+      <c r="B9" s="281"/>
       <c r="C9" s="202">
         <f>SUM(C28:C34)</f>
         <v>0</v>
@@ -25849,7 +25899,7 @@
       <c r="Y20" s="46"/>
     </row>
     <row r="21" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="282" t="s">
+      <c r="A21" s="277" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="208" t="s">
@@ -25917,7 +25967,7 @@
       <c r="W21" s="43"/>
     </row>
     <row r="22" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="282"/>
+      <c r="A22" s="277"/>
       <c r="B22" s="210" t="s">
         <v>3</v>
       </c>
@@ -25983,7 +26033,7 @@
       <c r="W22" s="43"/>
     </row>
     <row r="23" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="282"/>
+      <c r="A23" s="277"/>
       <c r="B23" s="210" t="s">
         <v>4</v>
       </c>
@@ -26049,7 +26099,7 @@
       <c r="W23" s="43"/>
     </row>
     <row r="24" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="282"/>
+      <c r="A24" s="277"/>
       <c r="B24" s="210" t="s">
         <v>5</v>
       </c>
@@ -26115,7 +26165,7 @@
       <c r="W24" s="43"/>
     </row>
     <row r="25" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="282"/>
+      <c r="A25" s="277"/>
       <c r="B25" s="210" t="s">
         <v>6</v>
       </c>
@@ -26181,7 +26231,7 @@
       <c r="W25" s="43"/>
     </row>
     <row r="26" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="282"/>
+      <c r="A26" s="277"/>
       <c r="B26" s="210" t="s">
         <v>7</v>
       </c>
@@ -26247,7 +26297,7 @@
       <c r="W26" s="43"/>
     </row>
     <row r="27" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="282"/>
+      <c r="A27" s="277"/>
       <c r="B27" s="208" t="s">
         <v>8</v>
       </c>
@@ -26313,7 +26363,7 @@
       <c r="W27" s="43"/>
     </row>
     <row r="28" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="282" t="s">
+      <c r="A28" s="277" t="s">
         <v>25</v>
       </c>
       <c r="B28" s="208" t="s">
@@ -26381,7 +26431,7 @@
       <c r="W28" s="43"/>
     </row>
     <row r="29" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="282"/>
+      <c r="A29" s="277"/>
       <c r="B29" s="210" t="s">
         <v>3</v>
       </c>
@@ -26447,7 +26497,7 @@
       <c r="W29" s="43"/>
     </row>
     <row r="30" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="282"/>
+      <c r="A30" s="277"/>
       <c r="B30" s="210" t="s">
         <v>4</v>
       </c>
@@ -26513,7 +26563,7 @@
       <c r="W30" s="43"/>
     </row>
     <row r="31" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="282"/>
+      <c r="A31" s="277"/>
       <c r="B31" s="210" t="s">
         <v>5</v>
       </c>
@@ -26579,7 +26629,7 @@
       <c r="W31" s="43"/>
     </row>
     <row r="32" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="282"/>
+      <c r="A32" s="277"/>
       <c r="B32" s="210" t="s">
         <v>6</v>
       </c>
@@ -26645,7 +26695,7 @@
       <c r="W32" s="43"/>
     </row>
     <row r="33" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="282"/>
+      <c r="A33" s="277"/>
       <c r="B33" s="210" t="s">
         <v>7</v>
       </c>
@@ -26711,7 +26761,7 @@
       <c r="W33" s="43"/>
     </row>
     <row r="34" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="282"/>
+      <c r="A34" s="277"/>
       <c r="B34" s="208" t="s">
         <v>8</v>
       </c>
@@ -26802,11 +26852,11 @@
     </row>
     <row r="36" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="203"/>
-      <c r="B36" s="287" t="s">
+      <c r="B36" s="282" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="287"/>
-      <c r="D36" s="287"/>
+      <c r="C36" s="282"/>
+      <c r="D36" s="282"/>
       <c r="E36" s="202"/>
       <c r="F36" s="202"/>
       <c r="G36" s="202"/>
@@ -30403,7 +30453,7 @@
         <v>1195</v>
       </c>
       <c r="W87" s="169"/>
-      <c r="X87" s="252"/>
+      <c r="X87" s="250"/>
       <c r="Y87" s="170"/>
     </row>
     <row r="88" spans="1:36" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -30471,7 +30521,7 @@
         <v>216</v>
       </c>
       <c r="W88" s="170"/>
-      <c r="X88" s="252"/>
+      <c r="X88" s="250"/>
       <c r="Y88" s="170"/>
     </row>
     <row r="89" spans="1:36" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -30539,7 +30589,7 @@
         <v>1383</v>
       </c>
       <c r="W89" s="170"/>
-      <c r="X89" s="252"/>
+      <c r="X89" s="250"/>
       <c r="Y89" s="170"/>
     </row>
     <row r="90" spans="1:36" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -30607,7 +30657,7 @@
         <v>1</v>
       </c>
       <c r="W90" s="170"/>
-      <c r="X90" s="252"/>
+      <c r="X90" s="250"/>
       <c r="Y90" s="170"/>
     </row>
     <row r="91" spans="1:36" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -30684,11 +30734,11 @@
       <c r="T93" s="13"/>
     </row>
     <row r="94" spans="1:36" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="294" t="s">
+      <c r="A94" s="290" t="s">
         <v>63</v>
       </c>
-      <c r="B94" s="294"/>
-      <c r="C94" s="294"/>
+      <c r="B94" s="290"/>
+      <c r="C94" s="290"/>
       <c r="D94" s="67"/>
       <c r="E94" s="64"/>
       <c r="F94" s="65"/>
@@ -30708,21 +30758,21 @@
       <c r="T94" s="13"/>
     </row>
     <row r="95" spans="1:36" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="291" t="s">
+      <c r="A95" s="286" t="s">
         <v>71</v>
       </c>
-      <c r="B95" s="291"/>
-      <c r="C95" s="291"/>
-      <c r="D95" s="291"/>
-      <c r="E95" s="291"/>
-      <c r="F95" s="291"/>
-      <c r="G95" s="291"/>
-      <c r="H95" s="291"/>
-      <c r="I95" s="291"/>
-      <c r="J95" s="291"/>
-      <c r="K95" s="291"/>
-      <c r="L95" s="291"/>
-      <c r="M95" s="291"/>
+      <c r="B95" s="286"/>
+      <c r="C95" s="286"/>
+      <c r="D95" s="286"/>
+      <c r="E95" s="286"/>
+      <c r="F95" s="286"/>
+      <c r="G95" s="286"/>
+      <c r="H95" s="286"/>
+      <c r="I95" s="286"/>
+      <c r="J95" s="286"/>
+      <c r="K95" s="286"/>
+      <c r="L95" s="286"/>
+      <c r="M95" s="286"/>
       <c r="N95" s="3"/>
       <c r="O95" s="3"/>
       <c r="P95" s="3"/>
@@ -30733,19 +30783,19 @@
       <c r="U95" s="3"/>
     </row>
     <row r="96" spans="1:36" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="291"/>
-      <c r="B96" s="291"/>
-      <c r="C96" s="291"/>
-      <c r="D96" s="291"/>
-      <c r="E96" s="291"/>
-      <c r="F96" s="291"/>
-      <c r="G96" s="291"/>
-      <c r="H96" s="291"/>
-      <c r="I96" s="291"/>
-      <c r="J96" s="291"/>
-      <c r="K96" s="291"/>
-      <c r="L96" s="291"/>
-      <c r="M96" s="291"/>
+      <c r="A96" s="286"/>
+      <c r="B96" s="286"/>
+      <c r="C96" s="286"/>
+      <c r="D96" s="286"/>
+      <c r="E96" s="286"/>
+      <c r="F96" s="286"/>
+      <c r="G96" s="286"/>
+      <c r="H96" s="286"/>
+      <c r="I96" s="286"/>
+      <c r="J96" s="286"/>
+      <c r="K96" s="286"/>
+      <c r="L96" s="286"/>
+      <c r="M96" s="286"/>
       <c r="N96" s="3"/>
       <c r="O96" s="3"/>
       <c r="P96" s="3"/>
@@ -30756,21 +30806,21 @@
       <c r="U96" s="3"/>
     </row>
     <row r="97" spans="1:20" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="290" t="s">
+      <c r="A97" s="285" t="s">
         <v>64</v>
       </c>
-      <c r="B97" s="290"/>
-      <c r="C97" s="290"/>
-      <c r="D97" s="290"/>
-      <c r="E97" s="290"/>
-      <c r="F97" s="290"/>
-      <c r="G97" s="290"/>
-      <c r="H97" s="290"/>
-      <c r="I97" s="290"/>
-      <c r="J97" s="290"/>
-      <c r="K97" s="290"/>
-      <c r="L97" s="290"/>
-      <c r="M97" s="290"/>
+      <c r="B97" s="285"/>
+      <c r="C97" s="285"/>
+      <c r="D97" s="285"/>
+      <c r="E97" s="285"/>
+      <c r="F97" s="285"/>
+      <c r="G97" s="285"/>
+      <c r="H97" s="285"/>
+      <c r="I97" s="285"/>
+      <c r="J97" s="285"/>
+      <c r="K97" s="285"/>
+      <c r="L97" s="285"/>
+      <c r="M97" s="285"/>
       <c r="N97" s="13"/>
       <c r="O97" s="13"/>
       <c r="P97" s="13"/>
@@ -30780,19 +30830,19 @@
       <c r="T97" s="13"/>
     </row>
     <row r="98" spans="1:20" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="290"/>
-      <c r="B98" s="290"/>
-      <c r="C98" s="290"/>
-      <c r="D98" s="290"/>
-      <c r="E98" s="290"/>
-      <c r="F98" s="290"/>
-      <c r="G98" s="290"/>
-      <c r="H98" s="290"/>
-      <c r="I98" s="290"/>
-      <c r="J98" s="290"/>
-      <c r="K98" s="290"/>
-      <c r="L98" s="290"/>
-      <c r="M98" s="290"/>
+      <c r="A98" s="285"/>
+      <c r="B98" s="285"/>
+      <c r="C98" s="285"/>
+      <c r="D98" s="285"/>
+      <c r="E98" s="285"/>
+      <c r="F98" s="285"/>
+      <c r="G98" s="285"/>
+      <c r="H98" s="285"/>
+      <c r="I98" s="285"/>
+      <c r="J98" s="285"/>
+      <c r="K98" s="285"/>
+      <c r="L98" s="285"/>
+      <c r="M98" s="285"/>
       <c r="N98" s="13"/>
       <c r="O98" s="13"/>
       <c r="P98" s="13"/>
@@ -30802,21 +30852,21 @@
       <c r="T98" s="13"/>
     </row>
     <row r="99" spans="1:20" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="289" t="s">
+      <c r="A99" s="284" t="s">
         <v>65</v>
       </c>
-      <c r="B99" s="289"/>
-      <c r="C99" s="289"/>
-      <c r="D99" s="289"/>
-      <c r="E99" s="289"/>
-      <c r="F99" s="289"/>
-      <c r="G99" s="289"/>
-      <c r="H99" s="289"/>
-      <c r="I99" s="289"/>
-      <c r="J99" s="289"/>
-      <c r="K99" s="289"/>
-      <c r="L99" s="289"/>
-      <c r="M99" s="289"/>
+      <c r="B99" s="284"/>
+      <c r="C99" s="284"/>
+      <c r="D99" s="284"/>
+      <c r="E99" s="284"/>
+      <c r="F99" s="284"/>
+      <c r="G99" s="284"/>
+      <c r="H99" s="284"/>
+      <c r="I99" s="284"/>
+      <c r="J99" s="284"/>
+      <c r="K99" s="284"/>
+      <c r="L99" s="284"/>
+      <c r="M99" s="284"/>
       <c r="N99" s="13"/>
       <c r="O99" s="13"/>
       <c r="P99" s="13"/>
@@ -30826,21 +30876,21 @@
       <c r="T99" s="13"/>
     </row>
     <row r="100" spans="1:20" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="290" t="s">
+      <c r="A100" s="285" t="s">
         <v>145</v>
       </c>
-      <c r="B100" s="290"/>
-      <c r="C100" s="290"/>
-      <c r="D100" s="290"/>
-      <c r="E100" s="290"/>
-      <c r="F100" s="290"/>
-      <c r="G100" s="290"/>
-      <c r="H100" s="290"/>
-      <c r="I100" s="290"/>
-      <c r="J100" s="290"/>
-      <c r="K100" s="290"/>
-      <c r="L100" s="290"/>
-      <c r="M100" s="290"/>
+      <c r="B100" s="285"/>
+      <c r="C100" s="285"/>
+      <c r="D100" s="285"/>
+      <c r="E100" s="285"/>
+      <c r="F100" s="285"/>
+      <c r="G100" s="285"/>
+      <c r="H100" s="285"/>
+      <c r="I100" s="285"/>
+      <c r="J100" s="285"/>
+      <c r="K100" s="285"/>
+      <c r="L100" s="285"/>
+      <c r="M100" s="285"/>
       <c r="N100" s="13"/>
       <c r="O100" s="13"/>
       <c r="P100" s="13"/>
@@ -30850,19 +30900,19 @@
       <c r="T100" s="13"/>
     </row>
     <row r="101" spans="1:20" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="290"/>
-      <c r="B101" s="290"/>
-      <c r="C101" s="290"/>
-      <c r="D101" s="290"/>
-      <c r="E101" s="290"/>
-      <c r="F101" s="290"/>
-      <c r="G101" s="290"/>
-      <c r="H101" s="290"/>
-      <c r="I101" s="290"/>
-      <c r="J101" s="290"/>
-      <c r="K101" s="290"/>
-      <c r="L101" s="290"/>
-      <c r="M101" s="290"/>
+      <c r="A101" s="285"/>
+      <c r="B101" s="285"/>
+      <c r="C101" s="285"/>
+      <c r="D101" s="285"/>
+      <c r="E101" s="285"/>
+      <c r="F101" s="285"/>
+      <c r="G101" s="285"/>
+      <c r="H101" s="285"/>
+      <c r="I101" s="285"/>
+      <c r="J101" s="285"/>
+      <c r="K101" s="285"/>
+      <c r="L101" s="285"/>
+      <c r="M101" s="285"/>
       <c r="N101" s="13"/>
       <c r="O101" s="13"/>
       <c r="P101" s="13"/>
@@ -30905,10 +30955,10 @@
       <c r="T103" s="13"/>
     </row>
     <row r="104" spans="1:20" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="288" t="s">
+      <c r="A104" s="283" t="s">
         <v>28</v>
       </c>
-      <c r="B104" s="288"/>
+      <c r="B104" s="283"/>
       <c r="C104" s="67"/>
       <c r="D104" s="67"/>
       <c r="E104" s="68"/>
@@ -30951,10 +31001,10 @@
       <c r="T105" s="13"/>
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A106" s="288" t="s">
+      <c r="A106" s="283" t="s">
         <v>66</v>
       </c>
-      <c r="B106" s="288"/>
+      <c r="B106" s="283"/>
       <c r="C106" s="29"/>
       <c r="D106" s="29"/>
       <c r="E106" s="29"/>
@@ -31001,8 +31051,8 @@
       <c r="B108" s="11"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
-      <c r="E108" s="281"/>
-      <c r="F108" s="281"/>
+      <c r="E108" s="276"/>
+      <c r="F108" s="276"/>
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
       <c r="I108" s="1"/>
@@ -31075,20 +31125,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="283" t="s">
+      <c r="A1" s="278" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="283"/>
-      <c r="C1" s="283"/>
-      <c r="D1" s="283"/>
-      <c r="E1" s="283"/>
-      <c r="F1" s="283"/>
-      <c r="G1" s="283"/>
+      <c r="B1" s="278"/>
+      <c r="C1" s="278"/>
+      <c r="D1" s="278"/>
+      <c r="E1" s="278"/>
+      <c r="F1" s="278"/>
+      <c r="G1" s="278"/>
       <c r="H1" s="32"/>
-      <c r="I1" s="304" t="s">
+      <c r="I1" s="297" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="304"/>
+      <c r="J1" s="297"/>
       <c r="K1" s="13"/>
       <c r="L1" s="13"/>
       <c r="M1" s="13"/>
@@ -31101,17 +31151,17 @@
       <c r="T1" s="53"/>
     </row>
     <row r="2" spans="1:23" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="305"/>
-      <c r="B2" s="305"/>
-      <c r="C2" s="305"/>
-      <c r="D2" s="305"/>
-      <c r="E2" s="305"/>
-      <c r="F2" s="305"/>
-      <c r="G2" s="305"/>
-      <c r="H2" s="305"/>
-      <c r="I2" s="305"/>
-      <c r="J2" s="305"/>
-      <c r="K2" s="305"/>
+      <c r="A2" s="298"/>
+      <c r="B2" s="298"/>
+      <c r="C2" s="298"/>
+      <c r="D2" s="298"/>
+      <c r="E2" s="298"/>
+      <c r="F2" s="298"/>
+      <c r="G2" s="298"/>
+      <c r="H2" s="298"/>
+      <c r="I2" s="298"/>
+      <c r="J2" s="298"/>
+      <c r="K2" s="298"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -31123,10 +31173,10 @@
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="284" t="s">
+      <c r="A3" s="279" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="284"/>
+      <c r="B3" s="279"/>
       <c r="C3" s="5">
         <v>1</v>
       </c>
@@ -31187,10 +31237,10 @@
       </c>
     </row>
     <row r="4" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="285" t="s">
+      <c r="A4" s="280" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="285"/>
+      <c r="B4" s="280"/>
       <c r="C4" s="6">
         <v>43829</v>
       </c>
@@ -31292,13 +31342,13 @@
       <c r="Q6" s="57"/>
       <c r="R6" s="57"/>
       <c r="S6" s="57"/>
-      <c r="T6" s="250"/>
+      <c r="T6" s="248"/>
     </row>
     <row r="7" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="306" t="s">
+      <c r="A7" s="299" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="306"/>
+      <c r="B7" s="299"/>
       <c r="C7" s="71">
         <v>1161</v>
       </c>
@@ -31360,10 +31410,10 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="306" t="s">
+      <c r="A8" s="299" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="306"/>
+      <c r="B8" s="299"/>
       <c r="C8" s="71">
         <f>SUM(C23:C29)</f>
         <v>616</v>
@@ -31442,10 +31492,10 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="306" t="s">
+      <c r="A9" s="299" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="306"/>
+      <c r="B9" s="299"/>
       <c r="C9" s="71">
         <f>SUM(C30:C36)</f>
         <v>545</v>
@@ -31588,10 +31638,10 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="285" t="s">
+      <c r="A11" s="280" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="285"/>
+      <c r="B11" s="280"/>
       <c r="C11" s="74"/>
       <c r="D11" s="74"/>
       <c r="E11" s="74"/>
@@ -32162,7 +32212,7 @@
       <c r="V22" s="45"/>
     </row>
     <row r="23" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="302" t="s">
+      <c r="A23" s="300" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="83" t="s">
@@ -32228,7 +32278,7 @@
       </c>
     </row>
     <row r="24" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="302"/>
+      <c r="A24" s="300"/>
       <c r="B24" s="84" t="s">
         <v>3</v>
       </c>
@@ -32292,7 +32342,7 @@
       </c>
     </row>
     <row r="25" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="302"/>
+      <c r="A25" s="300"/>
       <c r="B25" s="84" t="s">
         <v>4</v>
       </c>
@@ -32356,7 +32406,7 @@
       </c>
     </row>
     <row r="26" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="302"/>
+      <c r="A26" s="300"/>
       <c r="B26" s="84" t="s">
         <v>5</v>
       </c>
@@ -32420,7 +32470,7 @@
       </c>
     </row>
     <row r="27" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="302"/>
+      <c r="A27" s="300"/>
       <c r="B27" s="84" t="s">
         <v>6</v>
       </c>
@@ -32484,7 +32534,7 @@
       </c>
     </row>
     <row r="28" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="302"/>
+      <c r="A28" s="300"/>
       <c r="B28" s="84" t="s">
         <v>7</v>
       </c>
@@ -32548,7 +32598,7 @@
       </c>
     </row>
     <row r="29" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="302"/>
+      <c r="A29" s="300"/>
       <c r="B29" s="83" t="s">
         <v>8</v>
       </c>
@@ -32612,7 +32662,7 @@
       </c>
     </row>
     <row r="30" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="303" t="s">
+      <c r="A30" s="301" t="s">
         <v>25</v>
       </c>
       <c r="B30" s="83" t="s">
@@ -32678,7 +32728,7 @@
       </c>
     </row>
     <row r="31" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="303"/>
+      <c r="A31" s="301"/>
       <c r="B31" s="84" t="s">
         <v>3</v>
       </c>
@@ -32742,7 +32792,7 @@
       </c>
     </row>
     <row r="32" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="303"/>
+      <c r="A32" s="301"/>
       <c r="B32" s="84" t="s">
         <v>4</v>
       </c>
@@ -32806,7 +32856,7 @@
       </c>
     </row>
     <row r="33" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="303"/>
+      <c r="A33" s="301"/>
       <c r="B33" s="84" t="s">
         <v>5</v>
       </c>
@@ -32870,7 +32920,7 @@
       </c>
     </row>
     <row r="34" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="303"/>
+      <c r="A34" s="301"/>
       <c r="B34" s="84" t="s">
         <v>6</v>
       </c>
@@ -32934,7 +32984,7 @@
       </c>
     </row>
     <row r="35" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="303"/>
+      <c r="A35" s="301"/>
       <c r="B35" s="84" t="s">
         <v>7</v>
       </c>
@@ -32998,7 +33048,7 @@
       </c>
     </row>
     <row r="36" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="303"/>
+      <c r="A36" s="301"/>
       <c r="B36" s="83" t="s">
         <v>8</v>
       </c>
@@ -33085,11 +33135,11 @@
     </row>
     <row r="38" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="73"/>
-      <c r="B38" s="285" t="s">
+      <c r="B38" s="280" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="285"/>
-      <c r="D38" s="285"/>
+      <c r="C38" s="280"/>
+      <c r="D38" s="280"/>
       <c r="E38" s="70"/>
       <c r="F38" s="70"/>
       <c r="G38" s="70"/>
@@ -33106,23 +33156,23 @@
       <c r="R38" s="80"/>
       <c r="S38" s="80"/>
       <c r="T38" s="80"/>
-      <c r="X38" s="297"/>
-      <c r="Y38" s="297"/>
-      <c r="Z38" s="297"/>
-      <c r="AA38" s="297"/>
-      <c r="AB38" s="297"/>
-      <c r="AC38" s="297"/>
-      <c r="AD38" s="297"/>
-      <c r="AE38" s="297"/>
-      <c r="AF38" s="297"/>
-      <c r="AG38" s="297"/>
-      <c r="AH38" s="297"/>
-      <c r="AI38" s="297"/>
-      <c r="AJ38" s="297"/>
-      <c r="AK38" s="297"/>
-      <c r="AL38" s="297"/>
-      <c r="AM38" s="297"/>
-      <c r="AN38" s="297"/>
+      <c r="X38" s="292"/>
+      <c r="Y38" s="292"/>
+      <c r="Z38" s="292"/>
+      <c r="AA38" s="292"/>
+      <c r="AB38" s="292"/>
+      <c r="AC38" s="292"/>
+      <c r="AD38" s="292"/>
+      <c r="AE38" s="292"/>
+      <c r="AF38" s="292"/>
+      <c r="AG38" s="292"/>
+      <c r="AH38" s="292"/>
+      <c r="AI38" s="292"/>
+      <c r="AJ38" s="292"/>
+      <c r="AK38" s="292"/>
+      <c r="AL38" s="292"/>
+      <c r="AM38" s="292"/>
+      <c r="AN38" s="292"/>
     </row>
     <row r="39" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="48"/>
@@ -33187,23 +33237,23 @@
         <f>SUM(C39:T39)</f>
         <v>2000</v>
       </c>
-      <c r="X39" s="298"/>
-      <c r="Y39" s="298"/>
-      <c r="Z39" s="298"/>
-      <c r="AA39" s="298"/>
-      <c r="AB39" s="298"/>
-      <c r="AC39" s="298"/>
-      <c r="AD39" s="298"/>
-      <c r="AE39" s="298"/>
-      <c r="AF39" s="298"/>
-      <c r="AG39" s="298"/>
-      <c r="AH39" s="298"/>
-      <c r="AI39" s="298"/>
-      <c r="AJ39" s="298"/>
-      <c r="AK39" s="298"/>
-      <c r="AL39" s="298"/>
-      <c r="AM39" s="298"/>
-      <c r="AN39" s="298"/>
+      <c r="X39" s="293"/>
+      <c r="Y39" s="293"/>
+      <c r="Z39" s="293"/>
+      <c r="AA39" s="293"/>
+      <c r="AB39" s="293"/>
+      <c r="AC39" s="293"/>
+      <c r="AD39" s="293"/>
+      <c r="AE39" s="293"/>
+      <c r="AF39" s="293"/>
+      <c r="AG39" s="293"/>
+      <c r="AH39" s="293"/>
+      <c r="AI39" s="293"/>
+      <c r="AJ39" s="293"/>
+      <c r="AK39" s="293"/>
+      <c r="AL39" s="293"/>
+      <c r="AM39" s="293"/>
+      <c r="AN39" s="293"/>
       <c r="AO39" s="174"/>
       <c r="AP39" s="174"/>
       <c r="AQ39" s="174"/>
@@ -34548,23 +34598,23 @@
       <c r="U54" s="129"/>
       <c r="V54" s="126"/>
       <c r="W54" s="43"/>
-      <c r="X54" s="297"/>
-      <c r="Y54" s="297"/>
-      <c r="Z54" s="297"/>
-      <c r="AA54" s="297"/>
-      <c r="AB54" s="297"/>
-      <c r="AC54" s="297"/>
-      <c r="AD54" s="297"/>
-      <c r="AE54" s="297"/>
-      <c r="AF54" s="297"/>
-      <c r="AG54" s="297"/>
-      <c r="AH54" s="297"/>
-      <c r="AI54" s="297"/>
-      <c r="AJ54" s="297"/>
-      <c r="AK54" s="297"/>
-      <c r="AL54" s="297"/>
-      <c r="AM54" s="297"/>
-      <c r="AN54" s="297"/>
+      <c r="X54" s="292"/>
+      <c r="Y54" s="292"/>
+      <c r="Z54" s="292"/>
+      <c r="AA54" s="292"/>
+      <c r="AB54" s="292"/>
+      <c r="AC54" s="292"/>
+      <c r="AD54" s="292"/>
+      <c r="AE54" s="292"/>
+      <c r="AF54" s="292"/>
+      <c r="AG54" s="292"/>
+      <c r="AH54" s="292"/>
+      <c r="AI54" s="292"/>
+      <c r="AJ54" s="292"/>
+      <c r="AK54" s="292"/>
+      <c r="AL54" s="292"/>
+      <c r="AM54" s="292"/>
+      <c r="AN54" s="292"/>
       <c r="AO54" s="174"/>
     </row>
     <row r="55" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -34632,23 +34682,23 @@
         <v>881</v>
       </c>
       <c r="W55" s="43"/>
-      <c r="X55" s="298"/>
-      <c r="Y55" s="298"/>
-      <c r="Z55" s="298"/>
-      <c r="AA55" s="298"/>
-      <c r="AB55" s="298"/>
-      <c r="AC55" s="298"/>
-      <c r="AD55" s="298"/>
-      <c r="AE55" s="298"/>
-      <c r="AF55" s="298"/>
-      <c r="AG55" s="298"/>
-      <c r="AH55" s="298"/>
-      <c r="AI55" s="298"/>
-      <c r="AJ55" s="298"/>
-      <c r="AK55" s="298"/>
-      <c r="AL55" s="298"/>
-      <c r="AM55" s="298"/>
-      <c r="AN55" s="298"/>
+      <c r="X55" s="293"/>
+      <c r="Y55" s="293"/>
+      <c r="Z55" s="293"/>
+      <c r="AA55" s="293"/>
+      <c r="AB55" s="293"/>
+      <c r="AC55" s="293"/>
+      <c r="AD55" s="293"/>
+      <c r="AE55" s="293"/>
+      <c r="AF55" s="293"/>
+      <c r="AG55" s="293"/>
+      <c r="AH55" s="293"/>
+      <c r="AI55" s="293"/>
+      <c r="AJ55" s="293"/>
+      <c r="AK55" s="293"/>
+      <c r="AL55" s="293"/>
+      <c r="AM55" s="293"/>
+      <c r="AN55" s="293"/>
       <c r="AO55" s="174"/>
       <c r="AP55" s="174"/>
       <c r="AQ55" s="174"/>
@@ -38155,11 +38205,11 @@
       <c r="T95" s="53"/>
     </row>
     <row r="96" spans="1:57" s="54" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="294" t="s">
+      <c r="A96" s="290" t="s">
         <v>63</v>
       </c>
-      <c r="B96" s="294"/>
-      <c r="C96" s="294"/>
+      <c r="B96" s="290"/>
+      <c r="C96" s="290"/>
       <c r="D96" s="69"/>
       <c r="E96" s="89"/>
       <c r="F96" s="90"/>
@@ -38179,22 +38229,22 @@
       <c r="T96" s="53"/>
     </row>
     <row r="97" spans="1:20" s="54" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="291" t="s">
+      <c r="A97" s="286" t="s">
         <v>72</v>
       </c>
-      <c r="B97" s="291"/>
-      <c r="C97" s="291"/>
-      <c r="D97" s="291"/>
-      <c r="E97" s="291"/>
-      <c r="F97" s="291"/>
-      <c r="G97" s="291"/>
-      <c r="H97" s="291"/>
-      <c r="I97" s="291"/>
-      <c r="J97" s="291"/>
-      <c r="K97" s="291"/>
-      <c r="L97" s="291"/>
-      <c r="M97" s="291"/>
-      <c r="N97" s="291"/>
+      <c r="B97" s="286"/>
+      <c r="C97" s="286"/>
+      <c r="D97" s="286"/>
+      <c r="E97" s="286"/>
+      <c r="F97" s="286"/>
+      <c r="G97" s="286"/>
+      <c r="H97" s="286"/>
+      <c r="I97" s="286"/>
+      <c r="J97" s="286"/>
+      <c r="K97" s="286"/>
+      <c r="L97" s="286"/>
+      <c r="M97" s="286"/>
+      <c r="N97" s="286"/>
       <c r="O97" s="53"/>
       <c r="P97" s="53"/>
       <c r="Q97" s="53"/>
@@ -38203,20 +38253,20 @@
       <c r="T97" s="53"/>
     </row>
     <row r="98" spans="1:20" s="54" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="291"/>
-      <c r="B98" s="291"/>
-      <c r="C98" s="291"/>
-      <c r="D98" s="291"/>
-      <c r="E98" s="291"/>
-      <c r="F98" s="291"/>
-      <c r="G98" s="291"/>
-      <c r="H98" s="291"/>
-      <c r="I98" s="291"/>
-      <c r="J98" s="291"/>
-      <c r="K98" s="291"/>
-      <c r="L98" s="291"/>
-      <c r="M98" s="291"/>
-      <c r="N98" s="291"/>
+      <c r="A98" s="286"/>
+      <c r="B98" s="286"/>
+      <c r="C98" s="286"/>
+      <c r="D98" s="286"/>
+      <c r="E98" s="286"/>
+      <c r="F98" s="286"/>
+      <c r="G98" s="286"/>
+      <c r="H98" s="286"/>
+      <c r="I98" s="286"/>
+      <c r="J98" s="286"/>
+      <c r="K98" s="286"/>
+      <c r="L98" s="286"/>
+      <c r="M98" s="286"/>
+      <c r="N98" s="286"/>
       <c r="O98" s="53"/>
       <c r="P98" s="53"/>
       <c r="Q98" s="53"/>
@@ -38225,22 +38275,22 @@
       <c r="T98" s="53"/>
     </row>
     <row r="99" spans="1:20" s="54" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="290" t="s">
+      <c r="A99" s="285" t="s">
         <v>68</v>
       </c>
-      <c r="B99" s="290"/>
-      <c r="C99" s="290"/>
-      <c r="D99" s="290"/>
-      <c r="E99" s="290"/>
-      <c r="F99" s="290"/>
-      <c r="G99" s="290"/>
-      <c r="H99" s="290"/>
-      <c r="I99" s="290"/>
-      <c r="J99" s="290"/>
-      <c r="K99" s="290"/>
-      <c r="L99" s="290"/>
-      <c r="M99" s="290"/>
-      <c r="N99" s="290"/>
+      <c r="B99" s="285"/>
+      <c r="C99" s="285"/>
+      <c r="D99" s="285"/>
+      <c r="E99" s="285"/>
+      <c r="F99" s="285"/>
+      <c r="G99" s="285"/>
+      <c r="H99" s="285"/>
+      <c r="I99" s="285"/>
+      <c r="J99" s="285"/>
+      <c r="K99" s="285"/>
+      <c r="L99" s="285"/>
+      <c r="M99" s="285"/>
+      <c r="N99" s="285"/>
       <c r="O99" s="53"/>
       <c r="P99" s="53"/>
       <c r="Q99" s="53"/>
@@ -38249,20 +38299,20 @@
       <c r="T99" s="53"/>
     </row>
     <row r="100" spans="1:20" s="54" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="290"/>
-      <c r="B100" s="290"/>
-      <c r="C100" s="290"/>
-      <c r="D100" s="290"/>
-      <c r="E100" s="290"/>
-      <c r="F100" s="290"/>
-      <c r="G100" s="290"/>
-      <c r="H100" s="290"/>
-      <c r="I100" s="290"/>
-      <c r="J100" s="290"/>
-      <c r="K100" s="290"/>
-      <c r="L100" s="290"/>
-      <c r="M100" s="290"/>
-      <c r="N100" s="290"/>
+      <c r="A100" s="285"/>
+      <c r="B100" s="285"/>
+      <c r="C100" s="285"/>
+      <c r="D100" s="285"/>
+      <c r="E100" s="285"/>
+      <c r="F100" s="285"/>
+      <c r="G100" s="285"/>
+      <c r="H100" s="285"/>
+      <c r="I100" s="285"/>
+      <c r="J100" s="285"/>
+      <c r="K100" s="285"/>
+      <c r="L100" s="285"/>
+      <c r="M100" s="285"/>
+      <c r="N100" s="285"/>
       <c r="O100" s="53"/>
       <c r="P100" s="53"/>
       <c r="Q100" s="53"/>
@@ -38271,22 +38321,22 @@
       <c r="T100" s="53"/>
     </row>
     <row r="101" spans="1:20" s="54" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="290" t="s">
+      <c r="A101" s="285" t="s">
         <v>69</v>
       </c>
-      <c r="B101" s="300"/>
-      <c r="C101" s="300"/>
-      <c r="D101" s="300"/>
-      <c r="E101" s="300"/>
-      <c r="F101" s="300"/>
-      <c r="G101" s="300"/>
-      <c r="H101" s="300"/>
-      <c r="I101" s="300"/>
-      <c r="J101" s="300"/>
-      <c r="K101" s="300"/>
-      <c r="L101" s="300"/>
-      <c r="M101" s="300"/>
-      <c r="N101" s="300"/>
+      <c r="B101" s="295"/>
+      <c r="C101" s="295"/>
+      <c r="D101" s="295"/>
+      <c r="E101" s="295"/>
+      <c r="F101" s="295"/>
+      <c r="G101" s="295"/>
+      <c r="H101" s="295"/>
+      <c r="I101" s="295"/>
+      <c r="J101" s="295"/>
+      <c r="K101" s="295"/>
+      <c r="L101" s="295"/>
+      <c r="M101" s="295"/>
+      <c r="N101" s="295"/>
       <c r="O101" s="53"/>
       <c r="P101" s="53"/>
       <c r="Q101" s="53"/>
@@ -38295,20 +38345,20 @@
       <c r="T101" s="53"/>
     </row>
     <row r="102" spans="1:20" s="54" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="300"/>
-      <c r="B102" s="300"/>
-      <c r="C102" s="300"/>
-      <c r="D102" s="300"/>
-      <c r="E102" s="300"/>
-      <c r="F102" s="300"/>
-      <c r="G102" s="300"/>
-      <c r="H102" s="300"/>
-      <c r="I102" s="300"/>
-      <c r="J102" s="300"/>
-      <c r="K102" s="300"/>
-      <c r="L102" s="300"/>
-      <c r="M102" s="300"/>
-      <c r="N102" s="300"/>
+      <c r="A102" s="295"/>
+      <c r="B102" s="295"/>
+      <c r="C102" s="295"/>
+      <c r="D102" s="295"/>
+      <c r="E102" s="295"/>
+      <c r="F102" s="295"/>
+      <c r="G102" s="295"/>
+      <c r="H102" s="295"/>
+      <c r="I102" s="295"/>
+      <c r="J102" s="295"/>
+      <c r="K102" s="295"/>
+      <c r="L102" s="295"/>
+      <c r="M102" s="295"/>
+      <c r="N102" s="295"/>
       <c r="O102" s="53"/>
       <c r="P102" s="53"/>
       <c r="Q102" s="53"/>
@@ -38317,23 +38367,23 @@
       <c r="T102" s="53"/>
     </row>
     <row r="103" spans="1:20" s="54" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="290" t="s">
+      <c r="A103" s="285" t="s">
         <v>145</v>
       </c>
-      <c r="B103" s="290"/>
-      <c r="C103" s="290"/>
-      <c r="D103" s="290"/>
-      <c r="E103" s="290"/>
-      <c r="F103" s="290"/>
-      <c r="G103" s="290"/>
-      <c r="H103" s="290"/>
-      <c r="I103" s="290"/>
-      <c r="J103" s="290"/>
-      <c r="K103" s="290"/>
-      <c r="L103" s="290"/>
-      <c r="M103" s="290"/>
-      <c r="N103" s="290"/>
-      <c r="O103" s="290"/>
+      <c r="B103" s="285"/>
+      <c r="C103" s="285"/>
+      <c r="D103" s="285"/>
+      <c r="E103" s="285"/>
+      <c r="F103" s="285"/>
+      <c r="G103" s="285"/>
+      <c r="H103" s="285"/>
+      <c r="I103" s="285"/>
+      <c r="J103" s="285"/>
+      <c r="K103" s="285"/>
+      <c r="L103" s="285"/>
+      <c r="M103" s="285"/>
+      <c r="N103" s="285"/>
+      <c r="O103" s="285"/>
       <c r="P103" s="53"/>
       <c r="Q103" s="53"/>
       <c r="R103" s="53"/>
@@ -38369,8 +38419,8 @@
       <c r="B105" s="67"/>
       <c r="C105" s="63"/>
       <c r="D105" s="63"/>
-      <c r="E105" s="301"/>
-      <c r="F105" s="301"/>
+      <c r="E105" s="296"/>
+      <c r="F105" s="296"/>
       <c r="G105" s="30"/>
       <c r="H105" s="30"/>
       <c r="I105" s="30"/>
@@ -38387,10 +38437,10 @@
       <c r="T105" s="2"/>
     </row>
     <row r="106" spans="1:20" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="288" t="s">
+      <c r="A106" s="283" t="s">
         <v>28</v>
       </c>
-      <c r="B106" s="288"/>
+      <c r="B106" s="283"/>
       <c r="C106" s="94"/>
       <c r="D106" s="94"/>
       <c r="E106" s="94"/>
@@ -38405,10 +38455,10 @@
       <c r="N106" s="94"/>
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A108" s="288" t="s">
+      <c r="A108" s="283" t="s">
         <v>66</v>
       </c>
-      <c r="B108" s="299"/>
+      <c r="B108" s="294"/>
     </row>
   </sheetData>
   <mergeCells count="54">
@@ -38425,9 +38475,6 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A23:A29"/>
     <mergeCell ref="A30:A36"/>
-    <mergeCell ref="AJ38:AJ39"/>
-    <mergeCell ref="AC38:AC39"/>
-    <mergeCell ref="AD38:AD39"/>
     <mergeCell ref="AE38:AE39"/>
     <mergeCell ref="AF38:AF39"/>
     <mergeCell ref="AG38:AG39"/>
@@ -38443,6 +38490,12 @@
     <mergeCell ref="AD54:AD55"/>
     <mergeCell ref="AE54:AE55"/>
     <mergeCell ref="AF54:AF55"/>
+    <mergeCell ref="AK38:AK39"/>
+    <mergeCell ref="AI54:AI55"/>
+    <mergeCell ref="AJ54:AJ55"/>
+    <mergeCell ref="AJ38:AJ39"/>
+    <mergeCell ref="AC38:AC39"/>
+    <mergeCell ref="AD38:AD39"/>
     <mergeCell ref="A106:B106"/>
     <mergeCell ref="A108:B108"/>
     <mergeCell ref="A101:N102"/>
@@ -38451,21 +38504,18 @@
     <mergeCell ref="A99:N100"/>
     <mergeCell ref="A97:N98"/>
     <mergeCell ref="A103:O103"/>
-    <mergeCell ref="AL54:AL55"/>
-    <mergeCell ref="AM54:AM55"/>
-    <mergeCell ref="AN54:AN55"/>
-    <mergeCell ref="AM38:AM39"/>
-    <mergeCell ref="AN38:AN39"/>
     <mergeCell ref="AG54:AG55"/>
     <mergeCell ref="X54:X55"/>
     <mergeCell ref="Y54:Y55"/>
     <mergeCell ref="Z54:Z55"/>
     <mergeCell ref="AA54:AA55"/>
     <mergeCell ref="AB54:AB55"/>
-    <mergeCell ref="AK38:AK39"/>
+    <mergeCell ref="AL54:AL55"/>
+    <mergeCell ref="AM54:AM55"/>
+    <mergeCell ref="AN54:AN55"/>
+    <mergeCell ref="AM38:AM39"/>
+    <mergeCell ref="AN38:AN39"/>
     <mergeCell ref="AL38:AL39"/>
-    <mergeCell ref="AI54:AI55"/>
-    <mergeCell ref="AJ54:AJ55"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I1:J1" location="Contents!A1" display="back to contents"/>
@@ -38496,23 +38546,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="308" t="s">
+      <c r="A1" s="303" t="s">
         <v>165</v>
       </c>
-      <c r="B1" s="308"/>
-      <c r="C1" s="308"/>
-      <c r="D1" s="308"/>
-      <c r="E1" s="308"/>
-      <c r="F1" s="308"/>
-      <c r="G1" s="308"/>
-      <c r="H1" s="308"/>
-      <c r="I1" s="308"/>
-      <c r="J1" s="308"/>
-      <c r="K1" s="308"/>
-      <c r="M1" s="277" t="s">
+      <c r="B1" s="303"/>
+      <c r="C1" s="303"/>
+      <c r="D1" s="303"/>
+      <c r="E1" s="303"/>
+      <c r="F1" s="303"/>
+      <c r="G1" s="303"/>
+      <c r="H1" s="303"/>
+      <c r="I1" s="303"/>
+      <c r="J1" s="303"/>
+      <c r="K1" s="303"/>
+      <c r="M1" s="272" t="s">
         <v>70</v>
       </c>
-      <c r="N1" s="277"/>
+      <c r="N1" s="272"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="158"/>
@@ -38529,69 +38579,69 @@
     </row>
     <row r="3" spans="1:14" s="164" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="162"/>
-      <c r="B3" s="307" t="s">
+      <c r="B3" s="302" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="307"/>
-      <c r="D3" s="307"/>
-      <c r="E3" s="307"/>
-      <c r="F3" s="307"/>
+      <c r="C3" s="302"/>
+      <c r="D3" s="302"/>
+      <c r="E3" s="302"/>
+      <c r="F3" s="302"/>
       <c r="G3" s="163"/>
-      <c r="H3" s="307" t="s">
+      <c r="H3" s="302" t="s">
         <v>129</v>
       </c>
-      <c r="I3" s="307"/>
-      <c r="J3" s="307"/>
-      <c r="K3" s="307"/>
-      <c r="L3" s="307"/>
+      <c r="I3" s="302"/>
+      <c r="J3" s="302"/>
+      <c r="K3" s="302"/>
+      <c r="L3" s="302"/>
     </row>
     <row r="4" spans="1:14" s="164" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="162"/>
-      <c r="B4" s="328" t="s">
+      <c r="B4" s="308" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="328" t="s">
+      <c r="C4" s="308" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="330" t="s">
+      <c r="D4" s="310" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="328" t="s">
+      <c r="E4" s="308" t="s">
         <v>135</v>
       </c>
-      <c r="F4" s="328" t="s">
+      <c r="F4" s="308" t="s">
         <v>152</v>
       </c>
-      <c r="G4" s="331"/>
-      <c r="H4" s="328" t="s">
+      <c r="G4" s="312"/>
+      <c r="H4" s="308" t="s">
         <v>126</v>
       </c>
-      <c r="I4" s="328" t="s">
+      <c r="I4" s="308" t="s">
         <v>82</v>
       </c>
-      <c r="J4" s="330" t="s">
+      <c r="J4" s="310" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="328" t="s">
+      <c r="K4" s="308" t="s">
         <v>135</v>
       </c>
-      <c r="L4" s="328" t="s">
+      <c r="L4" s="308" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="164" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="165"/>
-      <c r="B5" s="327"/>
-      <c r="C5" s="327"/>
-      <c r="D5" s="329"/>
-      <c r="E5" s="327"/>
-      <c r="F5" s="327"/>
-      <c r="G5" s="332"/>
-      <c r="H5" s="327"/>
-      <c r="I5" s="327"/>
-      <c r="J5" s="329"/>
-      <c r="K5" s="327"/>
-      <c r="L5" s="327"/>
+      <c r="B5" s="309"/>
+      <c r="C5" s="309"/>
+      <c r="D5" s="311"/>
+      <c r="E5" s="309"/>
+      <c r="F5" s="309"/>
+      <c r="G5" s="313"/>
+      <c r="H5" s="309"/>
+      <c r="I5" s="309"/>
+      <c r="J5" s="311"/>
+      <c r="K5" s="309"/>
+      <c r="L5" s="309"/>
     </row>
     <row r="6" spans="1:14" s="164" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="162"/>
@@ -38633,23 +38683,23 @@
       <c r="G7" s="219"/>
       <c r="H7" s="219">
         <f>SUM(H10:H23)</f>
-        <v>5534</v>
+        <v>6729</v>
       </c>
       <c r="I7" s="219">
         <f t="shared" ref="I7:K7" si="1">SUM(I10:I23)</f>
-        <v>7041</v>
+        <v>7257</v>
       </c>
       <c r="J7" s="219">
         <f t="shared" si="1"/>
-        <v>9494</v>
+        <v>10877</v>
       </c>
       <c r="K7" s="219">
         <f t="shared" si="1"/>
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L7" s="219">
         <f>SUM(H7:K7)</f>
-        <v>22165</v>
+        <v>24960</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="164" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -38704,20 +38754,20 @@
       </c>
       <c r="G10" s="222"/>
       <c r="H10" s="222">
-        <v>413</v>
+        <v>499</v>
       </c>
       <c r="I10" s="222">
-        <v>554</v>
+        <v>573</v>
       </c>
       <c r="J10" s="222">
-        <v>839</v>
+        <v>926</v>
       </c>
       <c r="K10" s="222">
         <v>2</v>
       </c>
       <c r="L10" s="219">
         <f>SUM(H10:K10)</f>
-        <v>1808</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="164" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -38742,20 +38792,20 @@
       </c>
       <c r="G11" s="219"/>
       <c r="H11" s="219">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I11" s="219">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="J11" s="219">
-        <v>232</v>
+        <v>270</v>
       </c>
       <c r="K11" s="219">
         <v>49</v>
       </c>
       <c r="L11" s="219">
         <f t="shared" ref="L11:L23" si="3">SUM(H11:K11)</f>
-        <v>504</v>
+        <v>549</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="164" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -38780,20 +38830,20 @@
       </c>
       <c r="G12" s="219"/>
       <c r="H12" s="219">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="I12" s="219">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="J12" s="219">
-        <v>358</v>
+        <v>389</v>
       </c>
       <c r="K12" s="219">
         <v>0</v>
       </c>
       <c r="L12" s="219">
         <f t="shared" si="3"/>
-        <v>746</v>
+        <v>786</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="164" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -38818,20 +38868,20 @@
       </c>
       <c r="G13" s="219"/>
       <c r="H13" s="219">
-        <v>333</v>
+        <v>387</v>
       </c>
       <c r="I13" s="219">
-        <v>465</v>
+        <v>480</v>
       </c>
       <c r="J13" s="219">
-        <v>667</v>
+        <v>741</v>
       </c>
       <c r="K13" s="219">
         <v>0</v>
       </c>
       <c r="L13" s="219">
         <f t="shared" si="3"/>
-        <v>1465</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="164" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -38856,20 +38906,20 @@
       </c>
       <c r="G14" s="219"/>
       <c r="H14" s="219">
-        <v>342</v>
+        <v>411</v>
       </c>
       <c r="I14" s="219">
-        <v>392</v>
+        <v>407</v>
       </c>
       <c r="J14" s="219">
-        <v>503</v>
+        <v>575</v>
       </c>
       <c r="K14" s="219">
         <v>3</v>
       </c>
       <c r="L14" s="219">
         <f t="shared" si="3"/>
-        <v>1240</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="164" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -38894,20 +38944,20 @@
       </c>
       <c r="G15" s="219"/>
       <c r="H15" s="219">
-        <v>530</v>
+        <v>609</v>
       </c>
       <c r="I15" s="219">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="J15" s="219">
-        <v>990</v>
+        <v>1051</v>
       </c>
       <c r="K15" s="219">
         <v>2</v>
       </c>
       <c r="L15" s="219">
         <f t="shared" si="3"/>
-        <v>2173</v>
+        <v>2332</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="164" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -38932,20 +38982,20 @@
       </c>
       <c r="G16" s="219"/>
       <c r="H16" s="219">
-        <v>1305</v>
+        <v>1683</v>
       </c>
       <c r="I16" s="219">
-        <v>1559</v>
+        <v>1605</v>
       </c>
       <c r="J16" s="219">
-        <v>1897</v>
+        <v>2383</v>
       </c>
       <c r="K16" s="219">
         <v>11</v>
       </c>
       <c r="L16" s="219">
         <f t="shared" si="3"/>
-        <v>4772</v>
+        <v>5682</v>
       </c>
     </row>
     <row r="17" spans="1:12" s="164" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -38970,20 +39020,20 @@
       </c>
       <c r="G17" s="219"/>
       <c r="H17" s="219">
-        <v>334</v>
+        <v>358</v>
       </c>
       <c r="I17" s="219">
-        <v>485</v>
+        <v>498</v>
       </c>
       <c r="J17" s="219">
-        <v>567</v>
+        <v>618</v>
       </c>
       <c r="K17" s="219">
         <v>0</v>
       </c>
       <c r="L17" s="219">
         <f t="shared" si="3"/>
-        <v>1386</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="164" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -39008,20 +39058,20 @@
       </c>
       <c r="G18" s="219"/>
       <c r="H18" s="219">
-        <v>639</v>
+        <v>788</v>
       </c>
       <c r="I18" s="219">
-        <v>968</v>
+        <v>1004</v>
       </c>
       <c r="J18" s="219">
-        <v>1200</v>
+        <v>1399</v>
       </c>
       <c r="K18" s="219">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L18" s="219">
         <f t="shared" si="3"/>
-        <v>2818</v>
+        <v>3203</v>
       </c>
     </row>
     <row r="19" spans="1:12" s="164" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -39046,20 +39096,20 @@
       </c>
       <c r="G19" s="219"/>
       <c r="H19" s="219">
-        <v>851</v>
+        <v>1103</v>
       </c>
       <c r="I19" s="219">
-        <v>892</v>
+        <v>921</v>
       </c>
       <c r="J19" s="219">
-        <v>1318</v>
+        <v>1506</v>
       </c>
       <c r="K19" s="219">
         <v>0</v>
       </c>
       <c r="L19" s="219">
         <f t="shared" si="3"/>
-        <v>3061</v>
+        <v>3530</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="164" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -39090,14 +39140,14 @@
         <v>66</v>
       </c>
       <c r="J20" s="219">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K20" s="219">
         <v>0</v>
       </c>
       <c r="L20" s="219">
         <f t="shared" si="3"/>
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="164" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -39122,20 +39172,20 @@
       </c>
       <c r="G21" s="219"/>
       <c r="H21" s="219">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="I21" s="219">
         <v>19</v>
       </c>
       <c r="J21" s="219">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K21" s="219">
         <v>0</v>
       </c>
       <c r="L21" s="219">
         <f t="shared" si="3"/>
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="164" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -39160,20 +39210,20 @@
       </c>
       <c r="G22" s="219"/>
       <c r="H22" s="219">
-        <v>456</v>
+        <v>544</v>
       </c>
       <c r="I22" s="219">
-        <v>580</v>
+        <v>599</v>
       </c>
       <c r="J22" s="219">
-        <v>837</v>
+        <v>929</v>
       </c>
       <c r="K22" s="219">
         <v>18</v>
       </c>
       <c r="L22" s="219">
         <f t="shared" si="3"/>
-        <v>1891</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="164" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -40478,11 +40528,11 @@
       <c r="N59" s="146"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A60" s="309" t="s">
+      <c r="A60" s="304" t="s">
         <v>63</v>
       </c>
-      <c r="B60" s="309"/>
-      <c r="C60" s="309"/>
+      <c r="B60" s="304"/>
+      <c r="C60" s="304"/>
       <c r="D60" s="149"/>
       <c r="E60" s="145"/>
       <c r="F60" s="147"/>
@@ -40496,45 +40546,45 @@
       <c r="N60" s="146"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A61" s="311" t="s">
+      <c r="A61" s="306" t="s">
         <v>72</v>
       </c>
-      <c r="B61" s="311"/>
-      <c r="C61" s="311"/>
-      <c r="D61" s="311"/>
-      <c r="E61" s="311"/>
-      <c r="F61" s="311"/>
-      <c r="G61" s="311"/>
-      <c r="H61" s="311"/>
-      <c r="I61" s="311"/>
-      <c r="J61" s="311"/>
-      <c r="K61" s="311"/>
-      <c r="L61" s="311"/>
-      <c r="M61" s="311"/>
-      <c r="N61" s="311"/>
+      <c r="B61" s="306"/>
+      <c r="C61" s="306"/>
+      <c r="D61" s="306"/>
+      <c r="E61" s="306"/>
+      <c r="F61" s="306"/>
+      <c r="G61" s="306"/>
+      <c r="H61" s="306"/>
+      <c r="I61" s="306"/>
+      <c r="J61" s="306"/>
+      <c r="K61" s="306"/>
+      <c r="L61" s="306"/>
+      <c r="M61" s="306"/>
+      <c r="N61" s="306"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A62" s="311"/>
-      <c r="B62" s="311"/>
-      <c r="C62" s="311"/>
-      <c r="D62" s="311"/>
-      <c r="E62" s="311"/>
-      <c r="F62" s="311"/>
-      <c r="G62" s="311"/>
-      <c r="H62" s="311"/>
-      <c r="I62" s="311"/>
-      <c r="J62" s="311"/>
-      <c r="K62" s="311"/>
-      <c r="L62" s="311"/>
-      <c r="M62" s="311"/>
-      <c r="N62" s="311"/>
+      <c r="A62" s="306"/>
+      <c r="B62" s="306"/>
+      <c r="C62" s="306"/>
+      <c r="D62" s="306"/>
+      <c r="E62" s="306"/>
+      <c r="F62" s="306"/>
+      <c r="G62" s="306"/>
+      <c r="H62" s="306"/>
+      <c r="I62" s="306"/>
+      <c r="J62" s="306"/>
+      <c r="K62" s="306"/>
+      <c r="L62" s="306"/>
+      <c r="M62" s="306"/>
+      <c r="N62" s="306"/>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A63" s="309" t="s">
+      <c r="A63" s="304" t="s">
         <v>132</v>
       </c>
-      <c r="B63" s="309"/>
-      <c r="C63" s="309"/>
+      <c r="B63" s="304"/>
+      <c r="C63" s="304"/>
       <c r="D63" s="152"/>
       <c r="E63" s="152"/>
       <c r="F63" s="152"/>
@@ -40548,20 +40598,20 @@
       <c r="N63" s="152"/>
     </row>
     <row r="64" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="309" t="s">
+      <c r="A64" s="304" t="s">
         <v>144</v>
       </c>
-      <c r="B64" s="309"/>
-      <c r="C64" s="309"/>
-      <c r="D64" s="309"/>
-      <c r="E64" s="309"/>
-      <c r="F64" s="309"/>
-      <c r="G64" s="309"/>
-      <c r="H64" s="309"/>
-      <c r="I64" s="309"/>
-      <c r="J64" s="309"/>
-      <c r="K64" s="309"/>
-      <c r="L64" s="309"/>
+      <c r="B64" s="304"/>
+      <c r="C64" s="304"/>
+      <c r="D64" s="304"/>
+      <c r="E64" s="304"/>
+      <c r="F64" s="304"/>
+      <c r="G64" s="304"/>
+      <c r="H64" s="304"/>
+      <c r="I64" s="304"/>
+      <c r="J64" s="304"/>
+      <c r="K64" s="304"/>
+      <c r="L64" s="304"/>
       <c r="M64" s="151"/>
       <c r="N64" s="151"/>
     </row>
@@ -40570,8 +40620,8 @@
       <c r="B65" s="149"/>
       <c r="C65" s="145"/>
       <c r="D65" s="145"/>
-      <c r="E65" s="312"/>
-      <c r="F65" s="312"/>
+      <c r="E65" s="307"/>
+      <c r="F65" s="307"/>
       <c r="G65" s="150"/>
       <c r="H65" s="150"/>
       <c r="I65" s="150"/>
@@ -40582,10 +40632,10 @@
       <c r="N65" s="150"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A66" s="309" t="s">
+      <c r="A66" s="304" t="s">
         <v>28</v>
       </c>
-      <c r="B66" s="309"/>
+      <c r="B66" s="304"/>
       <c r="C66" s="142"/>
       <c r="D66" s="142"/>
       <c r="E66" s="142"/>
@@ -40616,10 +40666,10 @@
       <c r="N67" s="34"/>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A68" s="309" t="s">
+      <c r="A68" s="304" t="s">
         <v>66</v>
       </c>
-      <c r="B68" s="310"/>
+      <c r="B68" s="305"/>
       <c r="C68" s="34"/>
       <c r="D68" s="34"/>
       <c r="E68" s="34"/>
@@ -40681,24 +40731,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="314" t="s">
+      <c r="A1" s="315" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="314"/>
-      <c r="C1" s="314"/>
-      <c r="D1" s="314"/>
-      <c r="E1" s="314"/>
-      <c r="F1" s="314"/>
-      <c r="G1" s="314"/>
-      <c r="H1" s="314"/>
-      <c r="I1" s="314"/>
-      <c r="J1" s="314"/>
-      <c r="K1" s="314"/>
-      <c r="L1" s="314"/>
-      <c r="N1" s="313" t="s">
+      <c r="B1" s="315"/>
+      <c r="C1" s="315"/>
+      <c r="D1" s="315"/>
+      <c r="E1" s="315"/>
+      <c r="F1" s="315"/>
+      <c r="G1" s="315"/>
+      <c r="H1" s="315"/>
+      <c r="I1" s="315"/>
+      <c r="J1" s="315"/>
+      <c r="K1" s="315"/>
+      <c r="L1" s="315"/>
+      <c r="N1" s="314" t="s">
         <v>70</v>
       </c>
-      <c r="O1" s="313"/>
+      <c r="O1" s="314"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="98"/>
@@ -41258,10 +41308,10 @@
       <c r="E52" s="98"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="288" t="s">
+      <c r="A54" s="283" t="s">
         <v>66</v>
       </c>
-      <c r="B54" s="288"/>
+      <c r="B54" s="283"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -41292,24 +41342,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="314" t="s">
+      <c r="A1" s="315" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="314"/>
-      <c r="C1" s="314"/>
-      <c r="D1" s="314"/>
-      <c r="E1" s="314"/>
-      <c r="F1" s="314"/>
-      <c r="G1" s="314"/>
-      <c r="H1" s="314"/>
-      <c r="I1" s="314"/>
-      <c r="J1" s="314"/>
-      <c r="K1" s="314"/>
+      <c r="B1" s="315"/>
+      <c r="C1" s="315"/>
+      <c r="D1" s="315"/>
+      <c r="E1" s="315"/>
+      <c r="F1" s="315"/>
+      <c r="G1" s="315"/>
+      <c r="H1" s="315"/>
+      <c r="I1" s="315"/>
+      <c r="J1" s="315"/>
+      <c r="K1" s="315"/>
       <c r="L1" s="97"/>
-      <c r="M1" s="313" t="s">
+      <c r="M1" s="314" t="s">
         <v>70</v>
       </c>
-      <c r="N1" s="313"/>
+      <c r="N1" s="314"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="105"/>
@@ -42748,42 +42798,42 @@
       <c r="E109" s="98"/>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A110" s="309" t="s">
+      <c r="A110" s="304" t="s">
         <v>151</v>
       </c>
-      <c r="B110" s="309"/>
-      <c r="C110" s="309"/>
-      <c r="D110" s="309"/>
-      <c r="E110" s="309"/>
-      <c r="F110" s="309"/>
-      <c r="G110" s="309"/>
-      <c r="H110" s="309"/>
-      <c r="I110" s="309"/>
-      <c r="J110" s="309"/>
-      <c r="K110" s="309"/>
-      <c r="L110" s="309"/>
-      <c r="M110" s="309"/>
+      <c r="B110" s="304"/>
+      <c r="C110" s="304"/>
+      <c r="D110" s="304"/>
+      <c r="E110" s="304"/>
+      <c r="F110" s="304"/>
+      <c r="G110" s="304"/>
+      <c r="H110" s="304"/>
+      <c r="I110" s="304"/>
+      <c r="J110" s="304"/>
+      <c r="K110" s="304"/>
+      <c r="L110" s="304"/>
+      <c r="M110" s="304"/>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A111" s="257"/>
-      <c r="B111" s="257"/>
-      <c r="C111" s="257"/>
-      <c r="D111" s="257"/>
-      <c r="E111" s="257"/>
-      <c r="F111" s="257"/>
-      <c r="G111" s="257"/>
-      <c r="H111" s="257"/>
-      <c r="I111" s="257"/>
-      <c r="J111" s="257"/>
-      <c r="K111" s="257"/>
-      <c r="L111" s="257"/>
-      <c r="M111" s="257"/>
+      <c r="A111" s="255"/>
+      <c r="B111" s="255"/>
+      <c r="C111" s="255"/>
+      <c r="D111" s="255"/>
+      <c r="E111" s="255"/>
+      <c r="F111" s="255"/>
+      <c r="G111" s="255"/>
+      <c r="H111" s="255"/>
+      <c r="I111" s="255"/>
+      <c r="J111" s="255"/>
+      <c r="K111" s="255"/>
+      <c r="L111" s="255"/>
+      <c r="M111" s="255"/>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A112" s="288" t="s">
+      <c r="A112" s="283" t="s">
         <v>66</v>
       </c>
-      <c r="B112" s="288"/>
+      <c r="B112" s="283"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -42817,58 +42867,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="314" t="s">
+      <c r="A1" s="315" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="314"/>
-      <c r="C1" s="314"/>
-      <c r="D1" s="314"/>
-      <c r="E1" s="314"/>
-      <c r="F1" s="314"/>
-      <c r="G1" s="314"/>
-      <c r="H1" s="314"/>
+      <c r="B1" s="315"/>
+      <c r="C1" s="315"/>
+      <c r="D1" s="315"/>
+      <c r="E1" s="315"/>
+      <c r="F1" s="315"/>
+      <c r="G1" s="315"/>
+      <c r="H1" s="315"/>
       <c r="I1" s="97"/>
-      <c r="J1" s="316" t="s">
+      <c r="J1" s="317" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="316"/>
+      <c r="K1" s="317"/>
       <c r="L1" s="97"/>
       <c r="M1" s="110"/>
       <c r="N1" s="110"/>
     </row>
     <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="314" t="s">
+      <c r="A2" s="315" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="314"/>
-      <c r="C2" s="314"/>
-      <c r="D2" s="314"/>
-      <c r="E2" s="314"/>
-      <c r="F2" s="314"/>
-      <c r="G2" s="314"/>
+      <c r="B2" s="315"/>
+      <c r="C2" s="315"/>
+      <c r="D2" s="315"/>
+      <c r="E2" s="315"/>
+      <c r="F2" s="315"/>
+      <c r="G2" s="315"/>
       <c r="H2" s="97"/>
       <c r="I2" s="97"/>
       <c r="J2" s="97"/>
       <c r="K2" s="97"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="315"/>
-      <c r="B3" s="317" t="s">
+      <c r="A3" s="316"/>
+      <c r="B3" s="318" t="s">
         <v>76</v>
       </c>
       <c r="C3" s="105"/>
-      <c r="D3" s="317" t="s">
+      <c r="D3" s="318" t="s">
         <v>31</v>
       </c>
       <c r="E3" s="105"/>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="315"/>
-      <c r="B4" s="317"/>
+      <c r="A4" s="316"/>
+      <c r="B4" s="318"/>
       <c r="C4" s="107" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="317"/>
+      <c r="D4" s="318"/>
       <c r="E4" s="107" t="s">
         <v>77</v>
       </c>
@@ -43021,10 +43071,10 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="288" t="s">
+      <c r="A13" s="283" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="288"/>
+      <c r="B13" s="283"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -43067,20 +43117,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="318" t="s">
+      <c r="A1" s="319" t="s">
         <v>168</v>
       </c>
-      <c r="B1" s="318"/>
-      <c r="C1" s="318"/>
-      <c r="D1" s="318"/>
-      <c r="E1" s="318"/>
-      <c r="F1" s="318"/>
-      <c r="G1" s="318"/>
+      <c r="B1" s="319"/>
+      <c r="C1" s="319"/>
+      <c r="D1" s="319"/>
+      <c r="E1" s="319"/>
+      <c r="F1" s="319"/>
+      <c r="G1" s="319"/>
       <c r="H1" s="108"/>
-      <c r="I1" s="319" t="s">
+      <c r="I1" s="320" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="319"/>
+      <c r="J1" s="320"/>
       <c r="K1" s="108"/>
       <c r="L1" s="108"/>
       <c r="M1" s="108"/>
@@ -43103,17 +43153,17 @@
       <c r="N2" s="108"/>
     </row>
     <row r="3" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="259"/>
-      <c r="B3" s="317" t="s">
+      <c r="A3" s="257"/>
+      <c r="B3" s="318" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="317" t="s">
+      <c r="C3" s="318" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="317" t="s">
+      <c r="D3" s="318" t="s">
         <v>159</v>
       </c>
-      <c r="E3" s="317" t="s">
+      <c r="E3" s="318" t="s">
         <v>86</v>
       </c>
       <c r="F3" s="108"/>
@@ -43128,10 +43178,10 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="44"/>
-      <c r="B4" s="317"/>
-      <c r="C4" s="317"/>
-      <c r="D4" s="317"/>
-      <c r="E4" s="317"/>
+      <c r="B4" s="318"/>
+      <c r="C4" s="318"/>
+      <c r="D4" s="318"/>
+      <c r="E4" s="318"/>
       <c r="F4" s="136"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -43452,135 +43502,135 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="314" t="s">
+      <c r="A1" s="315" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="314"/>
-      <c r="C1" s="314"/>
-      <c r="D1" s="314"/>
-      <c r="E1" s="314"/>
-      <c r="G1" s="316" t="s">
+      <c r="B1" s="315"/>
+      <c r="C1" s="315"/>
+      <c r="D1" s="315"/>
+      <c r="E1" s="315"/>
+      <c r="G1" s="317" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="316"/>
+      <c r="H1" s="317"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="320" t="s">
+      <c r="A3" s="321" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="253" t="s">
+      <c r="B3" s="251" t="s">
         <v>195</v>
       </c>
-      <c r="C3" s="253" t="s">
+      <c r="C3" s="251" t="s">
         <v>196</v>
       </c>
-      <c r="D3" s="253" t="s">
+      <c r="D3" s="251" t="s">
         <v>197</v>
       </c>
-      <c r="E3" s="253" t="s">
+      <c r="E3" s="251" t="s">
         <v>198</v>
       </c>
-      <c r="F3" s="253" t="s">
+      <c r="F3" s="251" t="s">
         <v>199</v>
       </c>
-      <c r="G3" s="253" t="s">
+      <c r="G3" s="251" t="s">
         <v>200</v>
       </c>
-      <c r="H3" s="253" t="s">
+      <c r="H3" s="251" t="s">
         <v>201</v>
       </c>
-      <c r="I3" s="253" t="s">
+      <c r="I3" s="251" t="s">
         <v>202</v>
       </c>
-      <c r="J3" s="253" t="s">
+      <c r="J3" s="251" t="s">
         <v>203</v>
       </c>
-      <c r="K3" s="253" t="s">
+      <c r="K3" s="251" t="s">
         <v>204</v>
       </c>
-      <c r="L3" s="253" t="s">
+      <c r="L3" s="251" t="s">
         <v>205</v>
       </c>
-      <c r="M3" s="253" t="s">
+      <c r="M3" s="251" t="s">
         <v>206</v>
       </c>
-      <c r="N3" s="253" t="s">
+      <c r="N3" s="251" t="s">
         <v>207</v>
       </c>
-      <c r="O3" s="253" t="s">
+      <c r="O3" s="251" t="s">
         <v>208</v>
       </c>
-      <c r="P3" s="253" t="s">
+      <c r="P3" s="251" t="s">
         <v>209</v>
       </c>
-      <c r="Q3" s="253" t="s">
+      <c r="Q3" s="251" t="s">
         <v>210</v>
       </c>
-      <c r="R3" s="253" t="s">
+      <c r="R3" s="251" t="s">
         <v>211</v>
       </c>
-      <c r="S3" s="253" t="s">
+      <c r="S3" s="251" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A4" s="321"/>
-      <c r="B4" s="254" t="s">
+      <c r="A4" s="322"/>
+      <c r="B4" s="252" t="s">
         <v>178</v>
       </c>
-      <c r="C4" s="254" t="s">
+      <c r="C4" s="252" t="s">
         <v>177</v>
       </c>
-      <c r="D4" s="254" t="s">
+      <c r="D4" s="252" t="s">
         <v>179</v>
       </c>
-      <c r="E4" s="254" t="s">
+      <c r="E4" s="252" t="s">
         <v>180</v>
       </c>
-      <c r="F4" s="254" t="s">
+      <c r="F4" s="252" t="s">
         <v>181</v>
       </c>
-      <c r="G4" s="254" t="s">
+      <c r="G4" s="252" t="s">
         <v>182</v>
       </c>
-      <c r="H4" s="254" t="s">
+      <c r="H4" s="252" t="s">
         <v>183</v>
       </c>
-      <c r="I4" s="254" t="s">
+      <c r="I4" s="252" t="s">
         <v>184</v>
       </c>
-      <c r="J4" s="254" t="s">
+      <c r="J4" s="252" t="s">
         <v>185</v>
       </c>
-      <c r="K4" s="254" t="s">
+      <c r="K4" s="252" t="s">
         <v>186</v>
       </c>
-      <c r="L4" s="254" t="s">
+      <c r="L4" s="252" t="s">
         <v>187</v>
       </c>
-      <c r="M4" s="254" t="s">
+      <c r="M4" s="252" t="s">
         <v>188</v>
       </c>
-      <c r="N4" s="254" t="s">
+      <c r="N4" s="252" t="s">
         <v>189</v>
       </c>
-      <c r="O4" s="254" t="s">
+      <c r="O4" s="252" t="s">
         <v>190</v>
       </c>
-      <c r="P4" s="254" t="s">
+      <c r="P4" s="252" t="s">
         <v>191</v>
       </c>
-      <c r="Q4" s="254" t="s">
+      <c r="Q4" s="252" t="s">
         <v>192</v>
       </c>
-      <c r="R4" s="254" t="s">
+      <c r="R4" s="252" t="s">
         <v>193</v>
       </c>
-      <c r="S4" s="254" t="s">
+      <c r="S4" s="252" t="s">
         <v>194</v>
       </c>
-      <c r="T4" s="255"/>
+      <c r="T4" s="253"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="109" t="s">
@@ -43952,10 +44002,10 @@
       <c r="AA9" s="104"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A11" s="258" t="s">
+      <c r="A11" s="256" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="258"/>
+      <c r="B11" s="256"/>
     </row>
     <row r="27" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F27" s="105"/>

</xml_diff>